<commit_message>
finish simulations; make plots; minor enhancements
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_2_agile.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_2_agile.xlsx
@@ -730,90 +730,90 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>Oil retention [%]</t>
+          <t>Oil recovery [%]</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.01449076185963047</v>
+        <v>0.1564461153778446</v>
       </c>
       <c r="D4" t="n">
         <v>0.003529454733178189</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.03833437142137485</v>
+        <v>0.321833825577353</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.01530684090027363</v>
+        <v>-0.01530203168408126</v>
       </c>
       <c r="G4" t="n">
-        <v>0.007220401201342729</v>
+        <v>0.00109219051698201</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.0443029351161174</v>
+        <v>0.1032331694673642</v>
       </c>
       <c r="I4" t="n">
-        <v>0.00770345176413807</v>
+        <v>-0.02993212871728514</v>
       </c>
       <c r="J4" t="n">
-        <v>0.03550559258851486</v>
+        <v>-0.1028748494207504</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.02973551955742078</v>
+        <v>0.02208006808320272</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.02973551955742078</v>
+        <v>0.02208006808320272</v>
       </c>
       <c r="M4" t="n">
-        <v>-0.02973551955742078</v>
+        <v>0.02208006808320272</v>
       </c>
       <c r="N4" t="n">
-        <v>-0.02973551955742078</v>
+        <v>0.02208006808320272</v>
       </c>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="n">
-        <v>-0.0213915575916623</v>
+        <v>-0.02327832525113301</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.03168001883520075</v>
+        <v>0.03190542665221707</v>
       </c>
       <c r="R4" t="n">
-        <v>-0.03168001883520075</v>
+        <v>0.03190542665221707</v>
       </c>
       <c r="S4" t="n">
-        <v>-0.03168001883520075</v>
+        <v>0.03190542665221707</v>
       </c>
       <c r="T4" t="n">
-        <v>-0.03168001883520075</v>
+        <v>0.03190542665221707</v>
       </c>
       <c r="U4" t="n">
-        <v>-0.07360247632009903</v>
+        <v>0.2425557313982292</v>
       </c>
       <c r="V4" t="n">
-        <v>-0.4369569974462799</v>
+        <v>0.9735189411487576</v>
       </c>
       <c r="W4" t="n">
-        <v>0.01027472393098896</v>
+        <v>0.009795914311836572</v>
       </c>
       <c r="X4" t="n">
-        <v>-0.004733418975928386</v>
+        <v>-0.06157945336436114</v>
       </c>
       <c r="Y4" t="n">
-        <v>-0.01922797113711884</v>
+        <v>0.1160118957318398</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.07484190184167606</v>
+        <v>-0.1197627549985102</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.0005389885655595426</v>
+        <v>0.1208669360026774</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.0005389885655595426</v>
+        <v>0.1208669360026774</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.0005389885655595426</v>
+        <v>0.1208669360026774</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.0005389885655595426</v>
+        <v>0.1208669360026774</v>
       </c>
       <c r="AE4" t="inlineStr"/>
     </row>
@@ -821,90 +821,90 @@
       <c r="A5" s="1" t="n"/>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>Bagasse oil extraction efficiency [%]</t>
+          <t>Saccharification oil recovery [%]</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.07277556089502243</v>
+        <v>-0.002397055775882231</v>
       </c>
       <c r="D5" t="n">
         <v>0.007570266830810672</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1229394609815784</v>
+        <v>-0.05541093188043727</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.01142706381708255</v>
+        <v>-0.01142728298509132</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.01071776005134388</v>
+        <v>0.002789249439933099</v>
       </c>
       <c r="H5" t="n">
-        <v>0.04558606166344246</v>
+        <v>-0.0416371257284235</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.00535089727003589</v>
+        <v>0.0004415790896631636</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.03878848845673392</v>
+        <v>-0.004786033745015666</v>
       </c>
       <c r="K5" t="n">
-        <v>0.01199647977585919</v>
+        <v>-0.02664909994596399</v>
       </c>
       <c r="L5" t="n">
-        <v>0.01199647977585919</v>
+        <v>-0.02664909994596399</v>
       </c>
       <c r="M5" t="n">
-        <v>0.01199647977585919</v>
+        <v>-0.02664909994596399</v>
       </c>
       <c r="N5" t="n">
-        <v>0.01199647977585919</v>
+        <v>-0.02664909994596399</v>
       </c>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="n">
-        <v>-0.005383458455338337</v>
+        <v>-0.01670936303637452</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.01603616108944644</v>
+        <v>-0.02891349869253995</v>
       </c>
       <c r="R5" t="n">
-        <v>0.01603616108944644</v>
+        <v>-0.02891349869253995</v>
       </c>
       <c r="S5" t="n">
-        <v>0.01603616108944644</v>
+        <v>-0.02891349869253995</v>
       </c>
       <c r="T5" t="n">
-        <v>0.01603616108944644</v>
+        <v>-0.02891349869253995</v>
       </c>
       <c r="U5" t="n">
-        <v>0.08101435888857435</v>
+        <v>-0.05501886085675443</v>
       </c>
       <c r="V5" t="n">
-        <v>0.8408122722564908</v>
+        <v>-0.1867992094879684</v>
       </c>
       <c r="W5" t="n">
-        <v>0.0003160215486408619</v>
+        <v>0.0002029764561190582</v>
       </c>
       <c r="X5" t="n">
-        <v>-0.01525423226634396</v>
+        <v>0.01884669441105531</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.1724678091707123</v>
+        <v>-0.01231354641292732</v>
       </c>
       <c r="Z5" t="n">
-        <v>-0.009768306918732275</v>
+        <v>0.02722204467288178</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.1310658702346348</v>
+        <v>-0.01134899786195991</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.1310658702346348</v>
+        <v>-0.01134899786195991</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.1310658702346348</v>
+        <v>-0.01134899786195991</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.1310658702346348</v>
+        <v>-0.01134899786195991</v>
       </c>
       <c r="AE5" t="inlineStr"/>
     </row>
@@ -916,86 +916,86 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.1738102276244091</v>
+        <v>0.1736652329626093</v>
       </c>
       <c r="D6" t="n">
         <v>0.0108233524329341</v>
       </c>
       <c r="E6" t="n">
-        <v>0.006027640081105602</v>
+        <v>0.0009236422449456897</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.0006893062355722493</v>
+        <v>-0.0006891093395643735</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.01712317767251707</v>
+        <v>-0.0009457367892410298</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0001178903087156123</v>
+        <v>0.0003042623683088986</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.4508148372325935</v>
+        <v>-0.4497649716865988</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.03399475018798377</v>
+        <v>-0.002000616231370912</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.0005124210444968418</v>
+        <v>0.0001064440362577614</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.0005124210444968418</v>
+        <v>0.0001064440362577614</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.0005124210444968418</v>
+        <v>0.0001064440362577614</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.0005124210444968418</v>
+        <v>0.0001064440362577614</v>
       </c>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="n">
-        <v>-0.0008127527365101093</v>
+        <v>-0.0005441861977674478</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.000386627727465109</v>
+        <v>0.0001028573801142952</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.000386627727465109</v>
+        <v>0.0001028573801142952</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.000386627727465109</v>
+        <v>0.0001028573801142952</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.000386627727465109</v>
+        <v>0.0001028573801142952</v>
       </c>
       <c r="U6" t="n">
-        <v>0.0001962970638518825</v>
+        <v>-0.003764886294595452</v>
       </c>
       <c r="V6" t="n">
-        <v>0.0218979925559197</v>
+        <v>-0.002869433874777355</v>
       </c>
       <c r="W6" t="n">
-        <v>-0.01900365128814605</v>
+        <v>-0.01924619788984791</v>
       </c>
       <c r="X6" t="n">
-        <v>0.01415647556393152</v>
+        <v>-2.27868291367643e-05</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.01010163563606543</v>
+        <v>0.00884199836355477</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.02093405142936205</v>
+        <v>0.0209477026299081</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.005737772485510899</v>
+        <v>0.008441228593649142</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.005737772485510899</v>
+        <v>0.008441228593649142</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.005737772485510899</v>
+        <v>0.008441228593649142</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.005737772485510899</v>
+        <v>0.008441228593649142</v>
       </c>
       <c r="AE6" t="inlineStr"/>
     </row>
@@ -1007,86 +1007,86 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.07810599634023985</v>
+        <v>0.07199522371180894</v>
       </c>
       <c r="D7" t="n">
         <v>-0.004311911308476452</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.007426630665065225</v>
+        <v>-0.009782340199293606</v>
       </c>
       <c r="F7" t="n">
-        <v>0.001799452103978084</v>
+        <v>0.001798667879946715</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.01073018514205765</v>
+        <v>-0.02629031673707161</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.0003351532934061317</v>
+        <v>-0.001121676141077485</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.2293796710631868</v>
+        <v>-0.2283177426367097</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.01614282918549252</v>
+        <v>-0.0005077615421749621</v>
       </c>
       <c r="K7" t="n">
-        <v>0.001231079377243175</v>
+        <v>0.0003288205571528222</v>
       </c>
       <c r="L7" t="n">
-        <v>0.001231079377243175</v>
+        <v>0.0003288205571528222</v>
       </c>
       <c r="M7" t="n">
-        <v>0.001231079377243175</v>
+        <v>0.0003288205571528222</v>
       </c>
       <c r="N7" t="n">
-        <v>0.001231079377243175</v>
+        <v>0.0003288205571528222</v>
       </c>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="n">
-        <v>0.001724952932998117</v>
+        <v>0.002161173974446959</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.0009940778317631131</v>
+        <v>6.401280256051209e-05</v>
       </c>
       <c r="R7" t="n">
-        <v>0.0009940778317631131</v>
+        <v>6.401280256051209e-05</v>
       </c>
       <c r="S7" t="n">
-        <v>0.0009940778317631131</v>
+        <v>6.401280256051209e-05</v>
       </c>
       <c r="T7" t="n">
-        <v>0.0009940778317631131</v>
+        <v>6.401280256051209e-05</v>
       </c>
       <c r="U7" t="n">
-        <v>0.02308060517922421</v>
+        <v>0.01503491080939643</v>
       </c>
       <c r="V7" t="n">
-        <v>0.002079858419194336</v>
+        <v>-0.01395366209414648</v>
       </c>
       <c r="W7" t="n">
-        <v>0.01989632949985318</v>
+        <v>0.01991366978854679</v>
       </c>
       <c r="X7" t="n">
-        <v>-0.001083368623019399</v>
+        <v>0.02228452209971613</v>
       </c>
       <c r="Y7" t="n">
-        <v>-0.01737983723919349</v>
+        <v>-0.005704851915633534</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.0122049925521997</v>
+        <v>-0.008965704262628169</v>
       </c>
       <c r="AA7" t="n">
-        <v>-0.01197764303910572</v>
+        <v>-0.0065772900230916</v>
       </c>
       <c r="AB7" t="n">
-        <v>-0.01197764303910572</v>
+        <v>-0.0065772900230916</v>
       </c>
       <c r="AC7" t="n">
-        <v>-0.01197764303910572</v>
+        <v>-0.0065772900230916</v>
       </c>
       <c r="AD7" t="n">
-        <v>-0.01197764303910572</v>
+        <v>-0.0065772900230916</v>
       </c>
       <c r="AE7" t="inlineStr"/>
     </row>
@@ -1098,86 +1098,86 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.1888071824322873</v>
+        <v>0.1855737459189498</v>
       </c>
       <c r="D8" t="n">
         <v>0.9999999999999999</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.001377235927089437</v>
+        <v>-0.003075792795031711</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.002944693365787734</v>
+        <v>-0.002946490197859607</v>
       </c>
       <c r="G8" t="n">
-        <v>0.03269670657768003</v>
+        <v>0.0284369305702279</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.002140800181632007</v>
+        <v>0.001328822680859981</v>
       </c>
       <c r="I8" t="n">
-        <v>0.7721378912375155</v>
+        <v>0.7711386472615457</v>
       </c>
       <c r="J8" t="n">
-        <v>0.03321410268264075</v>
+        <v>0.008900613700707601</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.0005688011747520469</v>
+        <v>0.001971885294875411</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.0005688011747520469</v>
+        <v>0.001971885294875411</v>
       </c>
       <c r="M8" t="n">
-        <v>-0.0005688011747520469</v>
+        <v>0.001971885294875411</v>
       </c>
       <c r="N8" t="n">
-        <v>-0.0005688011747520469</v>
+        <v>0.001971885294875411</v>
       </c>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="n">
-        <v>-0.0001704983108199324</v>
+        <v>0.001370784150831366</v>
       </c>
       <c r="Q8" t="n">
-        <v>-0.0006622161864886473</v>
+        <v>0.002110037940401517</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.0006622161864886473</v>
+        <v>0.002110037940401517</v>
       </c>
       <c r="S8" t="n">
-        <v>-0.0006622161864886473</v>
+        <v>0.002110037940401517</v>
       </c>
       <c r="T8" t="n">
-        <v>-0.0006622161864886473</v>
+        <v>0.002110037940401517</v>
       </c>
       <c r="U8" t="n">
-        <v>-0.02814874634194985</v>
+        <v>-0.01076537678261507</v>
       </c>
       <c r="V8" t="n">
-        <v>-0.0004448660337946413</v>
+        <v>0.0007140504285620171</v>
       </c>
       <c r="W8" t="n">
-        <v>-0.02385954911438196</v>
+        <v>-0.02349211985168479</v>
       </c>
       <c r="X8" t="n">
-        <v>-0.003664017964009116</v>
+        <v>0.001502747953962546</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.005202932464117298</v>
+        <v>-0.01051825177943913</v>
       </c>
       <c r="Z8" t="n">
-        <v>-0.03065887975435519</v>
+        <v>-0.01702597834503913</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.004760166142406645</v>
+        <v>-0.01144687975387519</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.004760166142406645</v>
+        <v>-0.01144687975387519</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.004760166142406645</v>
+        <v>-0.01144687975387519</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.004760166142406645</v>
+        <v>-0.01144687975387519</v>
       </c>
       <c r="AE8" t="inlineStr"/>
     </row>
@@ -1193,86 +1193,86 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.6639215494688618</v>
+        <v>0.6659730426709216</v>
       </c>
       <c r="D9" t="n">
         <v>0.01752971628518865</v>
       </c>
       <c r="E9" t="n">
-        <v>0.002344032669761306</v>
+        <v>-0.00193221300528852</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.01370726416429056</v>
+        <v>-0.01370882157235286</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.02702443341727514</v>
+        <v>-0.009807260873283871</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.01803129374525175</v>
+        <v>-0.01858504607213561</v>
       </c>
       <c r="I9" t="n">
-        <v>0.003248652321946092</v>
+        <v>0.003082537179301487</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.01080910025367829</v>
+        <v>-0.03083900145880087</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.0152682324827293</v>
+        <v>-0.01642407905696316</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.0152682324827293</v>
+        <v>-0.01642407905696316</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.0152682324827293</v>
+        <v>-0.01642407905696316</v>
       </c>
       <c r="N9" t="n">
-        <v>-0.0152682324827293</v>
+        <v>-0.01642407905696316</v>
       </c>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="n">
-        <v>-0.01469212455568498</v>
+        <v>-0.01499086687163467</v>
       </c>
       <c r="Q9" t="n">
-        <v>-0.01572693461307738</v>
+        <v>-0.01683678547347142</v>
       </c>
       <c r="R9" t="n">
-        <v>-0.01572693461307738</v>
+        <v>-0.01683678547347142</v>
       </c>
       <c r="S9" t="n">
-        <v>-0.01572693461307738</v>
+        <v>-0.01683678547347142</v>
       </c>
       <c r="T9" t="n">
-        <v>-0.01572693461307738</v>
+        <v>-0.01683678547347142</v>
       </c>
       <c r="U9" t="n">
-        <v>-0.3795639974545598</v>
+        <v>-0.3171398613255945</v>
       </c>
       <c r="V9" t="n">
-        <v>0.005223330448933217</v>
+        <v>-0.004197360167894407</v>
       </c>
       <c r="W9" t="n">
-        <v>-0.01005661297826452</v>
+        <v>-0.01018586354343454</v>
       </c>
       <c r="X9" t="n">
-        <v>0.01958794300865036</v>
+        <v>0.009513660839875634</v>
       </c>
       <c r="Y9" t="n">
-        <v>-0.01443795984151839</v>
+        <v>-0.009416321904485738</v>
       </c>
       <c r="Z9" t="n">
-        <v>-0.006427877729115109</v>
+        <v>0.006427793633111745</v>
       </c>
       <c r="AA9" t="n">
-        <v>-0.007769577142783085</v>
+        <v>-0.01056153882246155</v>
       </c>
       <c r="AB9" t="n">
-        <v>-0.007769577142783085</v>
+        <v>-0.01056153882246155</v>
       </c>
       <c r="AC9" t="n">
-        <v>-0.007769577142783085</v>
+        <v>-0.01056153882246155</v>
       </c>
       <c r="AD9" t="n">
-        <v>-0.007769577142783085</v>
+        <v>-0.01056153882246155</v>
       </c>
       <c r="AE9" t="inlineStr"/>
     </row>
@@ -1288,86 +1288,86 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.3550122178484886</v>
+        <v>0.3311796221751848</v>
       </c>
       <c r="D10" t="n">
         <v>0.003197859583914383</v>
       </c>
       <c r="E10" t="n">
-        <v>0.03039465078378603</v>
+        <v>0.03094710987788439</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.03280610387224415</v>
+        <v>-0.03280650908826036</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.02024333632656823</v>
+        <v>-0.008225280841178304</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.03509710133988405</v>
+        <v>-0.0328428748136705</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.01863771021750841</v>
+        <v>-0.01974777976591119</v>
       </c>
       <c r="J10" t="n">
-        <v>0.004578455667554999</v>
+        <v>-0.00433268730921712</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.03617523619900944</v>
+        <v>-0.03420161340006453</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.03617523619900944</v>
+        <v>-0.03420161340006453</v>
       </c>
       <c r="M10" t="n">
-        <v>-0.03617523619900944</v>
+        <v>-0.03420161340006453</v>
       </c>
       <c r="N10" t="n">
-        <v>-0.03617523619900944</v>
+        <v>-0.03420161340006453</v>
       </c>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="n">
-        <v>-0.03580269618410784</v>
+        <v>-0.03529869481994779</v>
       </c>
       <c r="Q10" t="n">
-        <v>-0.03621950871278034</v>
+        <v>-0.03415726207029048</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.03621950871278034</v>
+        <v>-0.03415726207029048</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.03621950871278034</v>
+        <v>-0.03415726207029048</v>
       </c>
       <c r="T10" t="n">
-        <v>-0.03621950871278034</v>
+        <v>-0.03415726207029048</v>
       </c>
       <c r="U10" t="n">
-        <v>0.7456572247382889</v>
+        <v>0.5423473478378938</v>
       </c>
       <c r="V10" t="n">
-        <v>0.007453833610153343</v>
+        <v>0.001555266590210663</v>
       </c>
       <c r="W10" t="n">
-        <v>-0.01885870529834821</v>
+        <v>-0.01897474578298983</v>
       </c>
       <c r="X10" t="n">
-        <v>0.04343826143621506</v>
+        <v>0.01511660682105438</v>
       </c>
       <c r="Y10" t="n">
-        <v>-0.01038478419139137</v>
+        <v>0.01189532926308136</v>
       </c>
       <c r="Z10" t="n">
-        <v>-0.004407033872281355</v>
+        <v>0.02031520132460805</v>
       </c>
       <c r="AA10" t="n">
-        <v>-0.004472037298881491</v>
+        <v>0.01646443813057752</v>
       </c>
       <c r="AB10" t="n">
-        <v>-0.004472037298881491</v>
+        <v>0.01646443813057752</v>
       </c>
       <c r="AC10" t="n">
-        <v>-0.004472037298881491</v>
+        <v>0.01646443813057752</v>
       </c>
       <c r="AD10" t="n">
-        <v>-0.004472037298881491</v>
+        <v>0.01646443813057752</v>
       </c>
       <c r="AE10" t="inlineStr"/>
     </row>
@@ -1383,86 +1383,86 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-0.0008615281304611251</v>
+        <v>-0.05841131331245253</v>
       </c>
       <c r="D11" t="n">
         <v>0.007627171025086841</v>
       </c>
       <c r="E11" t="n">
-        <v>0.001292352627694105</v>
+        <v>-0.004934276741371069</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.0007660664946426597</v>
+        <v>-0.0007661096946443875</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.0005130542618994644</v>
+        <v>0.007956695471364903</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0004247555689902227</v>
+        <v>-0.006148718739593283</v>
       </c>
       <c r="I11" t="n">
-        <v>0.01465643281025731</v>
+        <v>0.014096525171861</v>
       </c>
       <c r="J11" t="n">
-        <v>0.0009176190151933433</v>
+        <v>-0.008898713092624598</v>
       </c>
       <c r="K11" t="n">
-        <v>-9.979699599187984e-05</v>
+        <v>-0.00352287652491506</v>
       </c>
       <c r="L11" t="n">
-        <v>-9.979699599187984e-05</v>
+        <v>-0.00352287652491506</v>
       </c>
       <c r="M11" t="n">
-        <v>-9.979699599187984e-05</v>
+        <v>-0.00352287652491506</v>
       </c>
       <c r="N11" t="n">
-        <v>-9.979699599187984e-05</v>
+        <v>-0.00352287652491506</v>
       </c>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="n">
-        <v>0.0002617038824681553</v>
+        <v>-0.001670281698811268</v>
       </c>
       <c r="Q11" t="n">
-        <v>3.299952131998085e-05</v>
+        <v>-0.003696876819875072</v>
       </c>
       <c r="R11" t="n">
-        <v>3.299952131998085e-05</v>
+        <v>-0.003696876819875072</v>
       </c>
       <c r="S11" t="n">
-        <v>3.299952131998085e-05</v>
+        <v>-0.003696876819875072</v>
       </c>
       <c r="T11" t="n">
-        <v>3.299952131998085e-05</v>
+        <v>-0.003696876819875072</v>
       </c>
       <c r="U11" t="n">
-        <v>-0.02404867401794696</v>
+        <v>0.1224424197136968</v>
       </c>
       <c r="V11" t="n">
-        <v>-0.00724087324963493</v>
+        <v>-0.0134103075444123</v>
       </c>
       <c r="W11" t="n">
-        <v>0.008976128519045138</v>
+        <v>0.008994535463781416</v>
       </c>
       <c r="X11" t="n">
-        <v>-0.006485122168338967</v>
+        <v>-0.007857933122560964</v>
       </c>
       <c r="Y11" t="n">
-        <v>-0.003149822813992912</v>
+        <v>0.005451779462209178</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.010521049956842</v>
+        <v>-0.01357342691093708</v>
       </c>
       <c r="AA11" t="n">
-        <v>-0.00889544656381786</v>
+        <v>0.0112356974094279</v>
       </c>
       <c r="AB11" t="n">
-        <v>-0.00889544656381786</v>
+        <v>0.0112356974094279</v>
       </c>
       <c r="AC11" t="n">
-        <v>-0.00889544656381786</v>
+        <v>0.0112356974094279</v>
       </c>
       <c r="AD11" t="n">
-        <v>-0.00889544656381786</v>
+        <v>0.0112356974094279</v>
       </c>
       <c r="AE11" t="inlineStr"/>
     </row>
@@ -1478,86 +1478,86 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-0.003564545230581809</v>
+        <v>-0.002099797043991881</v>
       </c>
       <c r="D12" t="n">
         <v>-0.004942293317691732</v>
       </c>
       <c r="E12" t="n">
-        <v>0.00866815330672613</v>
+        <v>0.01265797836231913</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.00233963452558538</v>
+        <v>-0.002339567805582712</v>
       </c>
       <c r="G12" t="n">
-        <v>0.009256205620119825</v>
+        <v>0.005734019507055594</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.00593171524526861</v>
+        <v>-0.003712928752764675</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.001594413471776538</v>
+        <v>-0.001420376024815041</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.01368230784839873</v>
+        <v>0.0003766606244495228</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.00737136855085474</v>
+        <v>-0.007160920414436815</v>
       </c>
       <c r="L12" t="n">
-        <v>-0.00737136855085474</v>
+        <v>-0.007160920414436815</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.00737136855085474</v>
+        <v>-0.007160920414436815</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.00737136855085474</v>
+        <v>-0.007160920414436815</v>
       </c>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="n">
-        <v>-0.007144834365793373</v>
+        <v>-0.007469230666769225</v>
       </c>
       <c r="Q12" t="n">
-        <v>-0.007412886632515465</v>
+        <v>-0.007030934297237371</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.007412886632515465</v>
+        <v>-0.007030934297237371</v>
       </c>
       <c r="S12" t="n">
-        <v>-0.007412886632515465</v>
+        <v>-0.007030934297237371</v>
       </c>
       <c r="T12" t="n">
-        <v>-0.007412886632515465</v>
+        <v>-0.007030934297237371</v>
       </c>
       <c r="U12" t="n">
-        <v>-0.002881919827276792</v>
+        <v>0.02195363876614555</v>
       </c>
       <c r="V12" t="n">
-        <v>-0.01107703397908136</v>
+        <v>0.009587708639508344</v>
       </c>
       <c r="W12" t="n">
-        <v>0.0119144650525786</v>
+        <v>0.0118715176268607</v>
       </c>
       <c r="X12" t="n">
-        <v>0.005028713950003646</v>
+        <v>-0.00871083311534252</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.02536632485465299</v>
+        <v>-0.01301928552529202</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.006839135793565431</v>
+        <v>-0.01741245919249837</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.01966554808262192</v>
+        <v>-0.009812400008496</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.01966554808262192</v>
+        <v>-0.009812400008496</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.01966554808262192</v>
+        <v>-0.009812400008496</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.01966554808262192</v>
+        <v>-0.009812400008496</v>
       </c>
       <c r="AE12" t="inlineStr"/>
     </row>
@@ -1569,86 +1569,86 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.2329817449992698</v>
+        <v>-0.2262524122820964</v>
       </c>
       <c r="D13" t="n">
         <v>-0.002908193588327743</v>
       </c>
       <c r="E13" t="n">
-        <v>0.01319959195198367</v>
+        <v>0.01940512589620503</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.007860968474438738</v>
+        <v>-0.007861038170441526</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.01599382058284482</v>
+        <v>-0.007911782414543525</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.007912716604508664</v>
+        <v>-0.00768122226350325</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.003036122425444896</v>
+        <v>-0.003964562174582486</v>
       </c>
       <c r="J13" t="n">
-        <v>0.003718093262807199</v>
+        <v>0.007709826048703523</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.009618498240739928</v>
+        <v>-0.01093403275736131</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.009618498240739928</v>
+        <v>-0.01093403275736131</v>
       </c>
       <c r="M13" t="n">
-        <v>-0.009618498240739928</v>
+        <v>-0.01093403275736131</v>
       </c>
       <c r="N13" t="n">
-        <v>-0.009618498240739928</v>
+        <v>-0.01093403275736131</v>
       </c>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="n">
-        <v>-0.009527079837083192</v>
+        <v>-0.01191694262067771</v>
       </c>
       <c r="Q13" t="n">
-        <v>-0.009392551959702077</v>
+        <v>-0.01057426170297047</v>
       </c>
       <c r="R13" t="n">
-        <v>-0.009392551959702077</v>
+        <v>-0.01057426170297047</v>
       </c>
       <c r="S13" t="n">
-        <v>-0.009392551959702077</v>
+        <v>-0.01057426170297047</v>
       </c>
       <c r="T13" t="n">
-        <v>-0.009392551959702077</v>
+        <v>-0.01057426170297047</v>
       </c>
       <c r="U13" t="n">
-        <v>0.003014892408595696</v>
+        <v>-0.009511098140443923</v>
       </c>
       <c r="V13" t="n">
-        <v>-0.01518431091137244</v>
+        <v>0.01303798832951953</v>
       </c>
       <c r="W13" t="n">
-        <v>0.005943911181756447</v>
+        <v>0.005914614956584598</v>
       </c>
       <c r="X13" t="n">
-        <v>0.02146872619162757</v>
+        <v>0.01230346106891601</v>
       </c>
       <c r="Y13" t="n">
-        <v>-0.004958290086331603</v>
+        <v>0.02591628868050092</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.01295650813426032</v>
+        <v>-0.01543893700155748</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.003119120860764834</v>
+        <v>0.02677157953486317</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.003119120860764834</v>
+        <v>0.02677157953486317</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.003119120860764834</v>
+        <v>0.02677157953486317</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.003119120860764834</v>
+        <v>0.02677157953486317</v>
       </c>
       <c r="AE13" t="inlineStr"/>
     </row>
@@ -1664,86 +1664,86 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.003132535037301401</v>
+        <v>0.003209873312394933</v>
       </c>
       <c r="D14" t="n">
         <v>-0.03053229702929188</v>
       </c>
       <c r="E14" t="n">
-        <v>0.005767629734705188</v>
+        <v>0.007088331163533246</v>
       </c>
       <c r="F14" t="n">
-        <v>0.003494376907775076</v>
+        <v>0.003497041195881648</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.03713812868871311</v>
+        <v>0.00862884346296902</v>
       </c>
       <c r="H14" t="n">
-        <v>0.006472409730896389</v>
+        <v>0.009509021273826874</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.02826485796259431</v>
+        <v>-0.02908655309946212</v>
       </c>
       <c r="J14" t="n">
-        <v>0.02723008397905134</v>
+        <v>0.02954009711407512</v>
       </c>
       <c r="K14" t="n">
-        <v>0.0043637200145488</v>
+        <v>0.007205769792230791</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0043637200145488</v>
+        <v>0.007205769792230791</v>
       </c>
       <c r="M14" t="n">
-        <v>0.0043637200145488</v>
+        <v>0.007205769792230791</v>
       </c>
       <c r="N14" t="n">
-        <v>0.0043637200145488</v>
+        <v>0.007205769792230791</v>
       </c>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="n">
-        <v>0.003515824556632982</v>
+        <v>0.005719374468774978</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.004674186234967449</v>
+        <v>0.007606191472247659</v>
       </c>
       <c r="R14" t="n">
-        <v>0.004674186234967449</v>
+        <v>0.007606191472247659</v>
       </c>
       <c r="S14" t="n">
-        <v>0.004674186234967449</v>
+        <v>0.007606191472247659</v>
       </c>
       <c r="T14" t="n">
-        <v>0.004674186234967449</v>
+        <v>0.007606191472247659</v>
       </c>
       <c r="U14" t="n">
-        <v>0.01973837858153514</v>
+        <v>0.02392908105316324</v>
       </c>
       <c r="V14" t="n">
-        <v>-0.01128154441926177</v>
+        <v>-0.002715854124634165</v>
       </c>
       <c r="W14" t="n">
-        <v>0.02126755774670231</v>
+        <v>0.02125158181006327</v>
       </c>
       <c r="X14" t="n">
-        <v>0.02618000202072573</v>
+        <v>-0.004641195395967038</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.02312592495703699</v>
+        <v>-0.003514382775706945</v>
       </c>
       <c r="Z14" t="n">
-        <v>-0.007519624908784996</v>
+        <v>0.009786633703465348</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.02519572929582917</v>
+        <v>-0.00336074375042975</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.02519572929582917</v>
+        <v>-0.00336074375042975</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.02519572929582917</v>
+        <v>-0.00336074375042975</v>
       </c>
       <c r="AD14" t="n">
-        <v>0.02519572929582917</v>
+        <v>-0.00336074375042975</v>
       </c>
       <c r="AE14" t="inlineStr"/>
     </row>
@@ -1759,86 +1759,86 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-0.01846154819446193</v>
+        <v>-0.01272781740511269</v>
       </c>
       <c r="D15" t="n">
         <v>0.002746113805844552</v>
       </c>
       <c r="E15" t="n">
-        <v>0.006272589178903566</v>
+        <v>0.003100364476014579</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.006617678952707157</v>
+        <v>-0.006620207880808314</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.009354200019329786</v>
+        <v>0.008154229162704219</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.006233513913340556</v>
+        <v>-0.004702719201966799</v>
       </c>
       <c r="I15" t="n">
-        <v>0.001713073124522925</v>
+        <v>0.002329485405179416</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.008375528229735561</v>
+        <v>-0.01420756535647279</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.005167422830696912</v>
+        <v>-0.003966838046673521</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.005167422830696912</v>
+        <v>-0.003966838046673521</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.005167422830696912</v>
+        <v>-0.003966838046673521</v>
       </c>
       <c r="N15" t="n">
-        <v>-0.005167422830696912</v>
+        <v>-0.003966838046673521</v>
       </c>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="n">
-        <v>-0.005875312843012513</v>
+        <v>-0.004715855324634212</v>
       </c>
       <c r="Q15" t="n">
-        <v>-0.005133271789330871</v>
+        <v>-0.003923054460922179</v>
       </c>
       <c r="R15" t="n">
-        <v>-0.005133271789330871</v>
+        <v>-0.003923054460922179</v>
       </c>
       <c r="S15" t="n">
-        <v>-0.005133271789330871</v>
+        <v>-0.003923054460922179</v>
       </c>
       <c r="T15" t="n">
-        <v>-0.005133271789330871</v>
+        <v>-0.003923054460922179</v>
       </c>
       <c r="U15" t="n">
-        <v>-0.04946697951467918</v>
+        <v>-0.04664875376995014</v>
       </c>
       <c r="V15" t="n">
-        <v>0.002217834520713381</v>
+        <v>0.001489720091588804</v>
       </c>
       <c r="W15" t="n">
-        <v>-0.008195136711805467</v>
+        <v>-0.008286053515442138</v>
       </c>
       <c r="X15" t="n">
-        <v>0.01994201690412866</v>
+        <v>-0.01222947276657242</v>
       </c>
       <c r="Y15" t="n">
-        <v>-0.003712745044509801</v>
+        <v>-3.461827711935102e-05</v>
       </c>
       <c r="Z15" t="n">
-        <v>-0.01494130350965214</v>
+        <v>0.0006139530485581219</v>
       </c>
       <c r="AA15" t="n">
-        <v>-0.008841008609640344</v>
+        <v>-0.00291165150846606</v>
       </c>
       <c r="AB15" t="n">
-        <v>-0.008841008609640344</v>
+        <v>-0.00291165150846606</v>
       </c>
       <c r="AC15" t="n">
-        <v>-0.008841008609640344</v>
+        <v>-0.00291165150846606</v>
       </c>
       <c r="AD15" t="n">
-        <v>-0.008841008609640344</v>
+        <v>-0.00291165150846606</v>
       </c>
       <c r="AE15" t="inlineStr"/>
     </row>
@@ -1854,86 +1854,86 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-0.01566379973055199</v>
+        <v>-0.01719588145583526</v>
       </c>
       <c r="D16" t="n">
         <v>-0.004229653321186132</v>
       </c>
       <c r="E16" t="n">
-        <v>0.002989581335583253</v>
+        <v>0.004140368133614724</v>
       </c>
       <c r="F16" t="n">
-        <v>0.004841014945640597</v>
+        <v>0.004840568833622753</v>
       </c>
       <c r="G16" t="n">
-        <v>0.005318562538709343</v>
+        <v>-0.006175730606227428</v>
       </c>
       <c r="H16" t="n">
-        <v>0.01126465581058623</v>
+        <v>0.01271272051096079</v>
       </c>
       <c r="I16" t="n">
-        <v>0.02241988236879529</v>
+        <v>0.02682629070505163</v>
       </c>
       <c r="J16" t="n">
-        <v>0.01618568296332289</v>
+        <v>0.03590087172786287</v>
       </c>
       <c r="K16" t="n">
-        <v>0.01107745551509822</v>
+        <v>0.01279455295978212</v>
       </c>
       <c r="L16" t="n">
-        <v>0.01107745551509822</v>
+        <v>0.01279455295978212</v>
       </c>
       <c r="M16" t="n">
-        <v>0.01107745551509822</v>
+        <v>0.01279455295978212</v>
       </c>
       <c r="N16" t="n">
-        <v>0.01107745551509822</v>
+        <v>0.01279455295978212</v>
       </c>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="n">
-        <v>0.009159862350394492</v>
+        <v>0.01052213072488523</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.01148265290730612</v>
+        <v>0.01323219739328789</v>
       </c>
       <c r="R16" t="n">
-        <v>0.01148265290730612</v>
+        <v>0.01323219739328789</v>
       </c>
       <c r="S16" t="n">
-        <v>0.01148265290730612</v>
+        <v>0.01323219739328789</v>
       </c>
       <c r="T16" t="n">
-        <v>0.01148265290730612</v>
+        <v>0.01323219739328789</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.004695117211804688</v>
+        <v>-0.008372405998896239</v>
       </c>
       <c r="V16" t="n">
-        <v>0.0007866799034671961</v>
+        <v>-7.893993915759755e-05</v>
       </c>
       <c r="W16" t="n">
-        <v>0.02052605918904237</v>
+        <v>0.02039124158364966</v>
       </c>
       <c r="X16" t="n">
-        <v>-0.004404894906209732</v>
+        <v>-0.03304199542099311</v>
       </c>
       <c r="Y16" t="n">
-        <v>-0.01146649073065963</v>
+        <v>-0.009216520386939087</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.09316653051066121</v>
+        <v>0.06853769698150787</v>
       </c>
       <c r="AA16" t="n">
-        <v>-0.003680252691210107</v>
+        <v>-0.008197578471903139</v>
       </c>
       <c r="AB16" t="n">
-        <v>-0.003680252691210107</v>
+        <v>-0.008197578471903139</v>
       </c>
       <c r="AC16" t="n">
-        <v>-0.003680252691210107</v>
+        <v>-0.008197578471903139</v>
       </c>
       <c r="AD16" t="n">
-        <v>-0.003680252691210107</v>
+        <v>-0.008197578471903139</v>
       </c>
       <c r="AE16" t="inlineStr"/>
     </row>
@@ -1949,86 +1949,86 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.07818572664742905</v>
+        <v>-0.07849303341172133</v>
       </c>
       <c r="D17" t="n">
         <v>0.001087392523495701</v>
       </c>
       <c r="E17" t="n">
-        <v>0.005268286290731451</v>
+        <v>0.006579801095192043</v>
       </c>
       <c r="F17" t="n">
-        <v>0.003101092732043709</v>
+        <v>0.003102832636113305</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.01984993381070193</v>
+        <v>-0.01911499817434947</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.002238244985529799</v>
+        <v>-0.003218904104347619</v>
       </c>
       <c r="I17" t="n">
-        <v>-0.006838617201544687</v>
+        <v>-0.007108364828334593</v>
       </c>
       <c r="J17" t="n">
-        <v>0.0009479369204882817</v>
+        <v>-0.01384720711673523</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.004070562882822515</v>
+        <v>-0.005038374345534973</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.004070562882822515</v>
+        <v>-0.005038374345534973</v>
       </c>
       <c r="M17" t="n">
-        <v>-0.004070562882822515</v>
+        <v>-0.005038374345534973</v>
       </c>
       <c r="N17" t="n">
-        <v>-0.004070562882822515</v>
+        <v>-0.005038374345534973</v>
       </c>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="n">
-        <v>-0.004513092084523682</v>
+        <v>-0.006190636279625451</v>
       </c>
       <c r="Q17" t="n">
-        <v>-0.00416494576659783</v>
+        <v>-0.005154305198172207</v>
       </c>
       <c r="R17" t="n">
-        <v>-0.00416494576659783</v>
+        <v>-0.005154305198172207</v>
       </c>
       <c r="S17" t="n">
-        <v>-0.00416494576659783</v>
+        <v>-0.005154305198172207</v>
       </c>
       <c r="T17" t="n">
-        <v>-0.00416494576659783</v>
+        <v>-0.005154305198172207</v>
       </c>
       <c r="U17" t="n">
-        <v>-0.06631720834868832</v>
+        <v>-0.0309925052077002</v>
       </c>
       <c r="V17" t="n">
-        <v>-0.0008789854431594176</v>
+        <v>0.008482843443313735</v>
       </c>
       <c r="W17" t="n">
-        <v>0.02576230384649215</v>
+        <v>0.02573260922130436</v>
       </c>
       <c r="X17" t="n">
-        <v>0.03061478236307125</v>
+        <v>-0.0009351172140173346</v>
       </c>
       <c r="Y17" t="n">
-        <v>0.03101567077662682</v>
+        <v>-0.01878879373848693</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.01343328149733126</v>
+        <v>0.001486140443445618</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.02506219069848763</v>
+        <v>-0.01703703936948157</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.02506219069848763</v>
+        <v>-0.01703703936948157</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.02506219069848763</v>
+        <v>-0.01703703936948157</v>
       </c>
       <c r="AD17" t="n">
-        <v>0.02506219069848763</v>
+        <v>-0.01703703936948157</v>
       </c>
       <c r="AE17" t="inlineStr"/>
     </row>
@@ -2040,86 +2040,86 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>-0.01148149917925997</v>
+        <v>-0.0005308529492341179</v>
       </c>
       <c r="D18" t="n">
         <v>1.123824044952962e-05</v>
       </c>
       <c r="E18" t="n">
-        <v>0.005417275128691004</v>
+        <v>0.02349971681198867</v>
       </c>
       <c r="F18" t="n">
-        <v>0.001798260359930414</v>
+        <v>0.001799136455965458</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.01227897347167663</v>
+        <v>-0.003591608217299711</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.001959461166378447</v>
+        <v>0.005219035631095447</v>
       </c>
       <c r="I18" t="n">
-        <v>-0.003060964346438573</v>
+        <v>-0.00488970125158805</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.006378173312424538</v>
+        <v>0.005498592624134538</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.003975874719034989</v>
+        <v>-0.001212054960482198</v>
       </c>
       <c r="L18" t="n">
-        <v>-0.003975874719034989</v>
+        <v>-0.001212054960482198</v>
       </c>
       <c r="M18" t="n">
-        <v>-0.003975874719034989</v>
+        <v>-0.001212054960482198</v>
       </c>
       <c r="N18" t="n">
-        <v>-0.003975874719034989</v>
+        <v>-0.001212054960482198</v>
       </c>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="n">
-        <v>-0.004260753674430146</v>
+        <v>-0.004687244059489762</v>
       </c>
       <c r="Q18" t="n">
-        <v>-0.003966471422658857</v>
+        <v>-0.0006408207616328303</v>
       </c>
       <c r="R18" t="n">
-        <v>-0.003966471422658857</v>
+        <v>-0.0006408207616328303</v>
       </c>
       <c r="S18" t="n">
-        <v>-0.003966471422658857</v>
+        <v>-0.0006408207616328303</v>
       </c>
       <c r="T18" t="n">
-        <v>-0.003966471422658857</v>
+        <v>-0.0006408207616328303</v>
       </c>
       <c r="U18" t="n">
-        <v>-0.02129281640371266</v>
+        <v>0.00998343975933759</v>
       </c>
       <c r="V18" t="n">
-        <v>-0.0336747327389893</v>
+        <v>0.04318150060726002</v>
       </c>
       <c r="W18" t="n">
-        <v>0.03200562944022518</v>
+        <v>0.03195348703813948</v>
       </c>
       <c r="X18" t="n">
-        <v>-0.003275577961183862</v>
+        <v>-0.00887142866777154</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.003888308411532336</v>
+        <v>-0.002408135780115133</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.03030914454036578</v>
+        <v>-0.009999012207960487</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.01176460664658426</v>
+        <v>0.003462357834494313</v>
       </c>
       <c r="AB18" t="n">
-        <v>0.01176460664658426</v>
+        <v>0.003462357834494313</v>
       </c>
       <c r="AC18" t="n">
-        <v>0.01176460664658426</v>
+        <v>0.003462357834494313</v>
       </c>
       <c r="AD18" t="n">
-        <v>0.01176460664658426</v>
+        <v>0.003462357834494313</v>
       </c>
       <c r="AE18" t="inlineStr"/>
     </row>
@@ -2135,86 +2135,86 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.03564919323396773</v>
+        <v>-0.03816003570240142</v>
       </c>
       <c r="D19" t="n">
         <v>0.005544996989799878</v>
       </c>
       <c r="E19" t="n">
-        <v>0.01786708468268339</v>
+        <v>0.01219782855191314</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.01350054457202178</v>
+        <v>-0.01350151340406053</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.008818374179807607</v>
+        <v>0.003949454963465461</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.00950249654009986</v>
+        <v>-0.01110784516375432</v>
       </c>
       <c r="I19" t="n">
-        <v>0.165044824873793</v>
+        <v>0.1605880886315235</v>
       </c>
       <c r="J19" t="n">
-        <v>0.003945028824500071</v>
+        <v>0.002932994480089735</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.01199488819179553</v>
+        <v>-0.010942924949717</v>
       </c>
       <c r="L19" t="n">
-        <v>-0.01199488819179553</v>
+        <v>-0.010942924949717</v>
       </c>
       <c r="M19" t="n">
-        <v>-0.01199488819179553</v>
+        <v>-0.010942924949717</v>
       </c>
       <c r="N19" t="n">
-        <v>-0.01199488819179553</v>
+        <v>-0.010942924949717</v>
       </c>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="n">
-        <v>-0.01232828948513158</v>
+        <v>-0.01171921938076877</v>
       </c>
       <c r="Q19" t="n">
-        <v>-0.01176124050244962</v>
+        <v>-0.01088199451527978</v>
       </c>
       <c r="R19" t="n">
-        <v>-0.01176124050244962</v>
+        <v>-0.01088199451527978</v>
       </c>
       <c r="S19" t="n">
-        <v>-0.01176124050244962</v>
+        <v>-0.01088199451527978</v>
       </c>
       <c r="T19" t="n">
-        <v>-0.01176124050244962</v>
+        <v>-0.01088199451527978</v>
       </c>
       <c r="U19" t="n">
-        <v>-0.01812735490109419</v>
+        <v>-0.01560227044809082</v>
       </c>
       <c r="V19" t="n">
-        <v>0.02051704814868192</v>
+        <v>-0.01096624066264962</v>
       </c>
       <c r="W19" t="n">
-        <v>0.001514493948579758</v>
+        <v>0.001633938113357524</v>
       </c>
       <c r="X19" t="n">
-        <v>-0.003883011858499954</v>
+        <v>0.001692619825475345</v>
       </c>
       <c r="Y19" t="n">
-        <v>0.01145814333832573</v>
+        <v>-0.004025553763298913</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.1144274775050991</v>
+        <v>0.07113598556543942</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.01255132207005288</v>
+        <v>-0.001311592948463718</v>
       </c>
       <c r="AB19" t="n">
-        <v>0.01255132207005288</v>
+        <v>-0.001311592948463718</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.01255132207005288</v>
+        <v>-0.001311592948463718</v>
       </c>
       <c r="AD19" t="n">
-        <v>0.01255132207005288</v>
+        <v>-0.001311592948463718</v>
       </c>
       <c r="AE19" t="inlineStr"/>
     </row>
@@ -2230,86 +2230,86 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>-0.009432091289283649</v>
+        <v>-0.008477379891095194</v>
       </c>
       <c r="D20" t="n">
         <v>-0.0007818678072747121</v>
       </c>
       <c r="E20" t="n">
-        <v>0.01185940713037629</v>
+        <v>0.01568102827524113</v>
       </c>
       <c r="F20" t="n">
-        <v>0.1091652696466108</v>
+        <v>0.109164475534579</v>
       </c>
       <c r="G20" t="n">
-        <v>0.01000600563173329</v>
+        <v>-0.005025201464708655</v>
       </c>
       <c r="H20" t="n">
-        <v>0.1051093200763728</v>
+        <v>0.1001531412003694</v>
       </c>
       <c r="I20" t="n">
-        <v>0.01440125184005007</v>
+        <v>0.01390786145231446</v>
       </c>
       <c r="J20" t="n">
-        <v>0.03016909031258218</v>
+        <v>0.02737560057154723</v>
       </c>
       <c r="K20" t="n">
-        <v>0.07460192784807711</v>
+        <v>0.07101932876077313</v>
       </c>
       <c r="L20" t="n">
-        <v>0.07460192784807711</v>
+        <v>0.07101932876077313</v>
       </c>
       <c r="M20" t="n">
-        <v>0.07460192784807711</v>
+        <v>0.07101932876077313</v>
       </c>
       <c r="N20" t="n">
-        <v>0.07460192784807711</v>
+        <v>0.07101932876077313</v>
       </c>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="n">
-        <v>0.0669875301995012</v>
+        <v>0.06372260213290408</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.07676270457450818</v>
+        <v>0.07315207041408281</v>
       </c>
       <c r="R20" t="n">
-        <v>0.07676270457450818</v>
+        <v>0.07315207041408281</v>
       </c>
       <c r="S20" t="n">
-        <v>0.07676270457450818</v>
+        <v>0.07315207041408281</v>
       </c>
       <c r="T20" t="n">
-        <v>0.07676270457450818</v>
+        <v>0.07315207041408281</v>
       </c>
       <c r="U20" t="n">
-        <v>0.02161883904075356</v>
+        <v>0.03264513144980525</v>
       </c>
       <c r="V20" t="n">
-        <v>-0.006481193923247756</v>
+        <v>0.01324404417776177</v>
       </c>
       <c r="W20" t="n">
-        <v>0.2859420223816809</v>
+        <v>0.2859784460311378</v>
       </c>
       <c r="X20" t="n">
-        <v>-0.02097764444295659</v>
+        <v>-0.01579847953078341</v>
       </c>
       <c r="Y20" t="n">
-        <v>0.03355112092604483</v>
+        <v>-0.01789534440636363</v>
       </c>
       <c r="Z20" t="n">
-        <v>0.006780598927223956</v>
+        <v>-0.04483612652944505</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.05752630166105206</v>
+        <v>-0.004415326448613058</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.05752630166105206</v>
+        <v>-0.004415326448613058</v>
       </c>
       <c r="AC20" t="n">
-        <v>0.05752630166105206</v>
+        <v>-0.004415326448613058</v>
       </c>
       <c r="AD20" t="n">
-        <v>0.05752630166105206</v>
+        <v>-0.004415326448613058</v>
       </c>
       <c r="AE20" t="inlineStr"/>
     </row>
@@ -2321,86 +2321,86 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>-0.01758923647956945</v>
+        <v>-0.01602408342496334</v>
       </c>
       <c r="D21" t="n">
         <v>0.002703635724145429</v>
       </c>
       <c r="E21" t="n">
-        <v>0.01809299073971963</v>
+        <v>0.01566725601869024</v>
       </c>
       <c r="F21" t="n">
-        <v>0.04144546994581879</v>
+        <v>0.04144419986576799</v>
       </c>
       <c r="G21" t="n">
-        <v>0.007624634828984744</v>
+        <v>-0.00595740522630821</v>
       </c>
       <c r="H21" t="n">
-        <v>0.03637917150316685</v>
+        <v>0.02958435130894893</v>
       </c>
       <c r="I21" t="n">
-        <v>0.04607908312316332</v>
+        <v>0.04374400744576029</v>
       </c>
       <c r="J21" t="n">
-        <v>0.0816009672293405</v>
+        <v>0.04772442458022107</v>
       </c>
       <c r="K21" t="n">
-        <v>0.02168064029122561</v>
+        <v>0.01608342160333686</v>
       </c>
       <c r="L21" t="n">
-        <v>0.02168064029122561</v>
+        <v>0.01608342160333686</v>
       </c>
       <c r="M21" t="n">
-        <v>0.02168064029122561</v>
+        <v>0.01608342160333686</v>
       </c>
       <c r="N21" t="n">
-        <v>0.02168064029122561</v>
+        <v>0.01608342160333686</v>
       </c>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="n">
-        <v>0.01765159923406397</v>
+        <v>0.01325875608235024</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.02253372723734908</v>
+        <v>0.01665762844230514</v>
       </c>
       <c r="R21" t="n">
-        <v>0.02253372723734908</v>
+        <v>0.01665762844230514</v>
       </c>
       <c r="S21" t="n">
-        <v>0.02253372723734908</v>
+        <v>0.01665762844230514</v>
       </c>
       <c r="T21" t="n">
-        <v>0.02253372723734908</v>
+        <v>0.01665762844230514</v>
       </c>
       <c r="U21" t="n">
-        <v>-0.001956892302275692</v>
+        <v>0.001010172520406901</v>
       </c>
       <c r="V21" t="n">
-        <v>0.004063898082555923</v>
+        <v>0.007427232585089302</v>
       </c>
       <c r="W21" t="n">
-        <v>0.1401599545343981</v>
+        <v>0.1401523891580956</v>
       </c>
       <c r="X21" t="n">
-        <v>-0.005236718264090562</v>
+        <v>-0.01641901891818418</v>
       </c>
       <c r="Y21" t="n">
-        <v>0.02875654953426198</v>
+        <v>0.0144061144983763</v>
       </c>
       <c r="Z21" t="n">
-        <v>0.009606941184277646</v>
+        <v>0.01069055706762228</v>
       </c>
       <c r="AA21" t="n">
-        <v>0.03506047541841901</v>
+        <v>0.01847091923483677</v>
       </c>
       <c r="AB21" t="n">
-        <v>0.03506047541841901</v>
+        <v>0.01847091923483677</v>
       </c>
       <c r="AC21" t="n">
-        <v>0.03506047541841901</v>
+        <v>0.01847091923483677</v>
       </c>
       <c r="AD21" t="n">
-        <v>0.03506047541841901</v>
+        <v>0.01847091923483677</v>
       </c>
       <c r="AE21" t="inlineStr"/>
     </row>
@@ -2412,86 +2412,86 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>-0.02198650398346016</v>
+        <v>-0.01993923410956936</v>
       </c>
       <c r="D22" t="n">
         <v>-0.007685123731404949</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.004735556829422272</v>
+        <v>-0.003441323081652923</v>
       </c>
       <c r="F22" t="n">
-        <v>0.1438543581061743</v>
+        <v>0.1438549535941981</v>
       </c>
       <c r="G22" t="n">
-        <v>0.001064563557775172</v>
+        <v>0.0167176138520213</v>
       </c>
       <c r="H22" t="n">
-        <v>0.1314234722649389</v>
+        <v>0.1211540572551233</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.00762287454491498</v>
+        <v>-0.007551379118055164</v>
       </c>
       <c r="J22" t="n">
-        <v>-0.003385265664591467</v>
+        <v>-0.006863920523761137</v>
       </c>
       <c r="K22" t="n">
-        <v>0.09480314654412585</v>
+        <v>0.0884089625123585</v>
       </c>
       <c r="L22" t="n">
-        <v>0.09480314654412585</v>
+        <v>0.0884089625123585</v>
       </c>
       <c r="M22" t="n">
-        <v>0.09480314654412585</v>
+        <v>0.0884089625123585</v>
       </c>
       <c r="N22" t="n">
-        <v>0.09480314654412585</v>
+        <v>0.0884089625123585</v>
       </c>
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="n">
-        <v>0.08789913135596523</v>
+        <v>0.08225050082602002</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.09690913530036539</v>
+        <v>0.09009147489965899</v>
       </c>
       <c r="R22" t="n">
-        <v>0.09690913530036539</v>
+        <v>0.09009147489965899</v>
       </c>
       <c r="S22" t="n">
-        <v>0.09690913530036539</v>
+        <v>0.09009147489965899</v>
       </c>
       <c r="T22" t="n">
-        <v>0.09690913530036539</v>
+        <v>0.09009147489965899</v>
       </c>
       <c r="U22" t="n">
-        <v>0.008192621415704855</v>
+        <v>0.01889608347584333</v>
       </c>
       <c r="V22" t="n">
-        <v>0.002777030703081228</v>
+        <v>-0.002016837488673499</v>
       </c>
       <c r="W22" t="n">
-        <v>0.3137275233331009</v>
+        <v>0.3137234641649385</v>
       </c>
       <c r="X22" t="n">
-        <v>-0.001524018522753937</v>
+        <v>-0.03804466203229784</v>
       </c>
       <c r="Y22" t="n">
-        <v>0.06013399238935968</v>
+        <v>-0.006074608546313146</v>
       </c>
       <c r="Z22" t="n">
-        <v>0.0330789953071598</v>
+        <v>-0.008276894443075776</v>
       </c>
       <c r="AA22" t="n">
-        <v>0.07469718058788723</v>
+        <v>0.006894744083789763</v>
       </c>
       <c r="AB22" t="n">
-        <v>0.07469718058788723</v>
+        <v>0.006894744083789763</v>
       </c>
       <c r="AC22" t="n">
-        <v>0.07469718058788723</v>
+        <v>0.006894744083789763</v>
       </c>
       <c r="AD22" t="n">
-        <v>0.07469718058788723</v>
+        <v>0.006894744083789763</v>
       </c>
       <c r="AE22" t="inlineStr"/>
     </row>
@@ -2503,86 +2503,86 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>-0.01162375419295017</v>
+        <v>-0.009748620677944825</v>
       </c>
       <c r="D23" t="n">
         <v>-0.001372140150885606</v>
       </c>
       <c r="E23" t="n">
-        <v>-0.008548805333952213</v>
+        <v>-0.01229206282768251</v>
       </c>
       <c r="F23" t="n">
-        <v>0.02327396867495874</v>
+        <v>0.02327487107499484</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.005855364231867829</v>
+        <v>-0.0006202811932935215</v>
       </c>
       <c r="H23" t="n">
-        <v>0.02184676676187067</v>
+        <v>0.01908689981020742</v>
       </c>
       <c r="I23" t="n">
-        <v>0.01294157091766284</v>
+        <v>0.01217007792680311</v>
       </c>
       <c r="J23" t="n">
-        <v>0.01143094426423849</v>
+        <v>0.004508938180914347</v>
       </c>
       <c r="K23" t="n">
-        <v>0.01863091082523643</v>
+        <v>0.01701810221672409</v>
       </c>
       <c r="L23" t="n">
-        <v>0.01863091082523643</v>
+        <v>0.01701810221672409</v>
       </c>
       <c r="M23" t="n">
-        <v>0.01863091082523643</v>
+        <v>0.01701810221672409</v>
       </c>
       <c r="N23" t="n">
-        <v>0.01863091082523643</v>
+        <v>0.01701810221672409</v>
       </c>
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="n">
-        <v>0.01731123198844927</v>
+        <v>0.01629405540376221</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.01883073848122954</v>
+        <v>0.0171426549257062</v>
       </c>
       <c r="R23" t="n">
-        <v>0.01883073848122954</v>
+        <v>0.0171426549257062</v>
       </c>
       <c r="S23" t="n">
-        <v>0.01883073848122954</v>
+        <v>0.0171426549257062</v>
       </c>
       <c r="T23" t="n">
-        <v>0.01883073848122954</v>
+        <v>0.0171426549257062</v>
       </c>
       <c r="U23" t="n">
-        <v>-0.01275287119811484</v>
+        <v>-0.01795933223837329</v>
       </c>
       <c r="V23" t="n">
-        <v>0.00802813577712543</v>
+        <v>-0.009339386677575464</v>
       </c>
       <c r="W23" t="n">
-        <v>0.03390136714805468</v>
+        <v>0.03383564986542599</v>
       </c>
       <c r="X23" t="n">
-        <v>-0.01790014276841993</v>
+        <v>0.003241106876214502</v>
       </c>
       <c r="Y23" t="n">
-        <v>0.0128772474590899</v>
+        <v>0.002741386485396249</v>
       </c>
       <c r="Z23" t="n">
-        <v>-0.03291930784477231</v>
+        <v>0.01313290420531617</v>
       </c>
       <c r="AA23" t="n">
-        <v>0.006679309035172361</v>
+        <v>0.003201037664041506</v>
       </c>
       <c r="AB23" t="n">
-        <v>0.006679309035172361</v>
+        <v>0.003201037664041506</v>
       </c>
       <c r="AC23" t="n">
-        <v>0.006679309035172361</v>
+        <v>0.003201037664041506</v>
       </c>
       <c r="AD23" t="n">
-        <v>0.006679309035172361</v>
+        <v>0.003201037664041506</v>
       </c>
       <c r="AE23" t="inlineStr"/>
     </row>
@@ -2598,86 +2598,86 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>-0.02217499048699962</v>
+        <v>-0.02176439232657569</v>
       </c>
       <c r="D24" t="n">
         <v>0.01651558885262355</v>
       </c>
       <c r="E24" t="n">
-        <v>0.006790529935621196</v>
+        <v>0.009482441947297676</v>
       </c>
       <c r="F24" t="n">
-        <v>0.1287280947491238</v>
+        <v>0.1287285824291433</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.01901674560728818</v>
+        <v>-0.004245362337642051</v>
       </c>
       <c r="H24" t="n">
-        <v>0.1228617883384715</v>
+        <v>0.1163244278503328</v>
       </c>
       <c r="I24" t="n">
-        <v>0.04583252554530102</v>
+        <v>0.04586807559472302</v>
       </c>
       <c r="J24" t="n">
-        <v>0.09178855904047294</v>
+        <v>0.0727760855622772</v>
       </c>
       <c r="K24" t="n">
-        <v>0.09002097912083915</v>
+        <v>0.08576088563843542</v>
       </c>
       <c r="L24" t="n">
-        <v>0.09002097912083915</v>
+        <v>0.08576088563843542</v>
       </c>
       <c r="M24" t="n">
-        <v>0.09002097912083915</v>
+        <v>0.08576088563843542</v>
       </c>
       <c r="N24" t="n">
-        <v>0.09002097912083915</v>
+        <v>0.08576088563843542</v>
       </c>
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="n">
-        <v>0.08176349981453999</v>
+        <v>0.07791975143679006</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.09237381441495256</v>
+        <v>0.0879844952313798</v>
       </c>
       <c r="R24" t="n">
-        <v>0.09237381441495256</v>
+        <v>0.0879844952313798</v>
       </c>
       <c r="S24" t="n">
-        <v>0.09237381441495256</v>
+        <v>0.0879844952313798</v>
       </c>
       <c r="T24" t="n">
-        <v>0.09237381441495256</v>
+        <v>0.0879844952313798</v>
       </c>
       <c r="U24" t="n">
-        <v>0.03140812368832494</v>
+        <v>0.03799372155174885</v>
       </c>
       <c r="V24" t="n">
-        <v>-0.01135575463023018</v>
+        <v>0.009757591398303653</v>
       </c>
       <c r="W24" t="n">
-        <v>-0.4948363780014551</v>
+        <v>-0.4948421653616866</v>
       </c>
       <c r="X24" t="n">
-        <v>0.01966311201353663</v>
+        <v>-0.03190884705959405</v>
       </c>
       <c r="Y24" t="n">
-        <v>-0.1519001811160072</v>
+        <v>-0.0784482462569271</v>
       </c>
       <c r="Z24" t="n">
-        <v>-0.06607969877118794</v>
+        <v>-0.06215772632630904</v>
       </c>
       <c r="AA24" t="n">
-        <v>-0.06518275729531028</v>
+        <v>-0.05036619820664792</v>
       </c>
       <c r="AB24" t="n">
-        <v>-0.06518275729531028</v>
+        <v>-0.05036619820664792</v>
       </c>
       <c r="AC24" t="n">
-        <v>-0.06518275729531028</v>
+        <v>-0.05036619820664792</v>
       </c>
       <c r="AD24" t="n">
-        <v>-0.06518275729531028</v>
+        <v>-0.05036619820664792</v>
       </c>
       <c r="AE24" t="inlineStr"/>
     </row>
@@ -2689,86 +2689,86 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>-0.008398969775958789</v>
+        <v>-0.006653072042122881</v>
       </c>
       <c r="D25" t="n">
         <v>-0.02022354388094175</v>
       </c>
       <c r="E25" t="n">
-        <v>0.01683269635330785</v>
+        <v>0.02220650056826002</v>
       </c>
       <c r="F25" t="n">
-        <v>0.2767957230078289</v>
+        <v>0.2767945667837826</v>
       </c>
       <c r="G25" t="n">
-        <v>0.007592102987824392</v>
+        <v>-0.02448358103709621</v>
       </c>
       <c r="H25" t="n">
-        <v>0.2476768854910754</v>
+        <v>0.2254370646083813</v>
       </c>
       <c r="I25" t="n">
-        <v>0.0409560551102422</v>
+        <v>0.03815548779821951</v>
       </c>
       <c r="J25" t="n">
-        <v>0.1200954221215157</v>
+        <v>0.05383440455905612</v>
       </c>
       <c r="K25" t="n">
-        <v>0.1763922491036899</v>
+        <v>0.1602731328749253</v>
       </c>
       <c r="L25" t="n">
-        <v>0.1763922491036899</v>
+        <v>0.1602731328749253</v>
       </c>
       <c r="M25" t="n">
-        <v>0.1763922491036899</v>
+        <v>0.1602731328749253</v>
       </c>
       <c r="N25" t="n">
-        <v>0.1763922491036899</v>
+        <v>0.1602731328749253</v>
       </c>
       <c r="O25" t="inlineStr"/>
       <c r="P25" t="n">
-        <v>0.1602468955938758</v>
+        <v>0.1458713126188525</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.1809486100219444</v>
+        <v>0.1640912552036502</v>
       </c>
       <c r="R25" t="n">
-        <v>0.1809486100219444</v>
+        <v>0.1640912552036502</v>
       </c>
       <c r="S25" t="n">
-        <v>0.1809486100219444</v>
+        <v>0.1640912552036502</v>
       </c>
       <c r="T25" t="n">
-        <v>0.1809486100219444</v>
+        <v>0.1640912552036502</v>
       </c>
       <c r="U25" t="n">
-        <v>0.01407831800313272</v>
+        <v>0.02111150638046025</v>
       </c>
       <c r="V25" t="n">
-        <v>-0.01957830692713227</v>
+        <v>0.01324732526589301</v>
       </c>
       <c r="W25" t="n">
-        <v>0.7177964202318567</v>
+        <v>0.7177960413198415</v>
       </c>
       <c r="X25" t="n">
-        <v>-0.03135424214271309</v>
+        <v>-0.05787379410602142</v>
       </c>
       <c r="Y25" t="n">
-        <v>0.0984884906915396</v>
+        <v>0.01257377581141004</v>
       </c>
       <c r="Z25" t="n">
-        <v>0.04295658824626353</v>
+        <v>0.01365261433810457</v>
       </c>
       <c r="AA25" t="n">
-        <v>0.1427568688782747</v>
+        <v>0.04240261302410452</v>
       </c>
       <c r="AB25" t="n">
-        <v>0.1427568688782747</v>
+        <v>0.04240261302410452</v>
       </c>
       <c r="AC25" t="n">
-        <v>0.1427568688782747</v>
+        <v>0.04240261302410452</v>
       </c>
       <c r="AD25" t="n">
-        <v>0.1427568688782747</v>
+        <v>0.04240261302410452</v>
       </c>
       <c r="AE25" t="inlineStr"/>
     </row>
@@ -2784,86 +2784,86 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.1791128235485129</v>
+        <v>0.2075284036291361</v>
       </c>
       <c r="D26" t="n">
         <v>-0.01490230658009226</v>
       </c>
       <c r="E26" t="n">
-        <v>0.01913056319722253</v>
+        <v>0.02248856806754272</v>
       </c>
       <c r="F26" t="n">
-        <v>-0.02472371292494852</v>
+        <v>-0.02472246962889878</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.03019404595620929</v>
+        <v>-0.01039632432173874</v>
       </c>
       <c r="H26" t="n">
-        <v>-0.2387568593742743</v>
+        <v>-0.2986039467289345</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.2854049628401985</v>
+        <v>-0.2923900923676037</v>
       </c>
       <c r="J26" t="n">
-        <v>-0.6528454951163367</v>
+        <v>-0.6498322837554754</v>
       </c>
       <c r="K26" t="n">
-        <v>-0.239718851220754</v>
+        <v>-0.3080528437781138</v>
       </c>
       <c r="L26" t="n">
-        <v>-0.239718851220754</v>
+        <v>-0.3080528437781138</v>
       </c>
       <c r="M26" t="n">
-        <v>-0.239718851220754</v>
+        <v>-0.3080528437781138</v>
       </c>
       <c r="N26" t="n">
-        <v>-0.239718851220754</v>
+        <v>-0.3080528437781138</v>
       </c>
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="n">
-        <v>-0.2153415899256636</v>
+        <v>-0.2749581844383273</v>
       </c>
       <c r="Q26" t="n">
-        <v>-0.2480675714267028</v>
+        <v>-0.3179248886849955</v>
       </c>
       <c r="R26" t="n">
-        <v>-0.2480675714267028</v>
+        <v>-0.3179248886849955</v>
       </c>
       <c r="S26" t="n">
-        <v>-0.2480675714267028</v>
+        <v>-0.3179248886849955</v>
       </c>
       <c r="T26" t="n">
-        <v>-0.2480675714267028</v>
+        <v>-0.3179248886849955</v>
       </c>
       <c r="U26" t="n">
-        <v>-0.2219455234058209</v>
+        <v>-0.1057661379906455</v>
       </c>
       <c r="V26" t="n">
-        <v>0.01439752243190089</v>
+        <v>0.01619673069586923</v>
       </c>
       <c r="W26" t="n">
-        <v>0.02402745782509831</v>
+        <v>0.0239714474868579</v>
       </c>
       <c r="X26" t="n">
-        <v>-0.00655908756035084</v>
+        <v>0.04558262130156296</v>
       </c>
       <c r="Y26" t="n">
-        <v>0.3639756967350278</v>
+        <v>0.131137667520639</v>
       </c>
       <c r="Z26" t="n">
-        <v>0.3267273542530941</v>
+        <v>0.2047848648313945</v>
       </c>
       <c r="AA26" t="n">
-        <v>0.3028200731688029</v>
+        <v>0.1537191224687649</v>
       </c>
       <c r="AB26" t="n">
-        <v>0.3028200731688029</v>
+        <v>0.1537191224687649</v>
       </c>
       <c r="AC26" t="n">
-        <v>0.3028200731688029</v>
+        <v>0.1537191224687649</v>
       </c>
       <c r="AD26" t="n">
-        <v>0.3028200731688029</v>
+        <v>0.1537191224687649</v>
       </c>
       <c r="AE26" t="inlineStr"/>
     </row>
@@ -2875,86 +2875,86 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.02545740322629612</v>
+        <v>0.02392108434884337</v>
       </c>
       <c r="D27" t="n">
         <v>0.01960177316807092</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.01173824629352985</v>
+        <v>-0.01357917875116715</v>
       </c>
       <c r="F27" t="n">
-        <v>0.01956340321453613</v>
+        <v>0.01956149915045996</v>
       </c>
       <c r="G27" t="n">
-        <v>0.02273596511169864</v>
+        <v>-0.02367338934231262</v>
       </c>
       <c r="H27" t="n">
-        <v>0.02273469921338797</v>
+        <v>0.02266081650159051</v>
       </c>
       <c r="I27" t="n">
-        <v>-0.04075725167829006</v>
+        <v>-0.04021057946442318</v>
       </c>
       <c r="J27" t="n">
-        <v>0.01162513369653271</v>
+        <v>0.01476746301292464</v>
       </c>
       <c r="K27" t="n">
-        <v>0.02093326950933078</v>
+        <v>0.02111817098872684</v>
       </c>
       <c r="L27" t="n">
-        <v>0.02093326950933078</v>
+        <v>0.02111817098872684</v>
       </c>
       <c r="M27" t="n">
-        <v>0.02093326950933078</v>
+        <v>0.02111817098872684</v>
       </c>
       <c r="N27" t="n">
-        <v>0.02093326950933078</v>
+        <v>0.02111817098872684</v>
       </c>
       <c r="O27" t="inlineStr"/>
       <c r="P27" t="n">
-        <v>0.02046434779457391</v>
+        <v>0.02120520123220804</v>
       </c>
       <c r="Q27" t="n">
-        <v>0.02119890286395611</v>
+        <v>0.02136142914245716</v>
       </c>
       <c r="R27" t="n">
-        <v>0.02119890286395611</v>
+        <v>0.02136142914245716</v>
       </c>
       <c r="S27" t="n">
-        <v>0.02119890286395611</v>
+        <v>0.02136142914245716</v>
       </c>
       <c r="T27" t="n">
-        <v>0.02119890286395611</v>
+        <v>0.02136142914245716</v>
       </c>
       <c r="U27" t="n">
-        <v>-0.006831102417244096</v>
+        <v>-0.01699470519178821</v>
       </c>
       <c r="V27" t="n">
-        <v>-0.0005739669349586773</v>
+        <v>-0.009719331076773242</v>
       </c>
       <c r="W27" t="n">
-        <v>-0.00326750576270023</v>
+        <v>-0.003285680771427231</v>
       </c>
       <c r="X27" t="n">
-        <v>-0.02228008387126658</v>
+        <v>0.03201458202269743</v>
       </c>
       <c r="Y27" t="n">
-        <v>-0.007693835827753431</v>
+        <v>-0.005247660248024028</v>
       </c>
       <c r="Z27" t="n">
-        <v>0.09125821123432844</v>
+        <v>0.07077733175909326</v>
       </c>
       <c r="AA27" t="n">
-        <v>0.001723331300933252</v>
+        <v>-0.00377126952685078</v>
       </c>
       <c r="AB27" t="n">
-        <v>0.001723331300933252</v>
+        <v>-0.00377126952685078</v>
       </c>
       <c r="AC27" t="n">
-        <v>0.001723331300933252</v>
+        <v>-0.00377126952685078</v>
       </c>
       <c r="AD27" t="n">
-        <v>0.001723331300933252</v>
+        <v>-0.00377126952685078</v>
       </c>
       <c r="AE27" t="inlineStr"/>
     </row>
@@ -2970,86 +2970,86 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>-0.0118593551943742</v>
+        <v>-0.007772136118885444</v>
       </c>
       <c r="D28" t="n">
         <v>0.01176916271076651</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.06006970425878816</v>
+        <v>-0.04812063187682526</v>
       </c>
       <c r="F28" t="n">
-        <v>0.03263010399320416</v>
+        <v>0.0326300451452018</v>
       </c>
       <c r="G28" t="n">
-        <v>0.001362332620480502</v>
+        <v>0.02575514991381168</v>
       </c>
       <c r="H28" t="n">
-        <v>0.00397652377506095</v>
+        <v>0.01144186177835207</v>
       </c>
       <c r="I28" t="n">
-        <v>0.02437551812702072</v>
+        <v>0.02372972888518915</v>
       </c>
       <c r="J28" t="n">
-        <v>0.005519641195754914</v>
+        <v>-0.001195179412195875</v>
       </c>
       <c r="K28" t="n">
-        <v>0.01428242044329681</v>
+        <v>0.01870046599601864</v>
       </c>
       <c r="L28" t="n">
-        <v>0.01428242044329681</v>
+        <v>0.01870046599601864</v>
       </c>
       <c r="M28" t="n">
-        <v>0.01428242044329681</v>
+        <v>0.01870046599601864</v>
       </c>
       <c r="N28" t="n">
-        <v>0.01428242044329681</v>
+        <v>0.01870046599601864</v>
       </c>
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="n">
-        <v>0.02097337178293487</v>
+        <v>0.02320185443207417</v>
       </c>
       <c r="Q28" t="n">
-        <v>0.01275271548610862</v>
+        <v>0.01757035212681408</v>
       </c>
       <c r="R28" t="n">
-        <v>0.01275271548610862</v>
+        <v>0.01757035212681408</v>
       </c>
       <c r="S28" t="n">
-        <v>0.01275271548610862</v>
+        <v>0.01757035212681408</v>
       </c>
       <c r="T28" t="n">
-        <v>0.01275271548610862</v>
+        <v>0.01757035212681408</v>
       </c>
       <c r="U28" t="n">
-        <v>-0.04636957212678288</v>
+        <v>-0.02508700785148031</v>
       </c>
       <c r="V28" t="n">
-        <v>-0.2806375019455</v>
+        <v>-0.09119297068771881</v>
       </c>
       <c r="W28" t="n">
-        <v>0.04827231236289249</v>
+        <v>0.04818086544723461</v>
       </c>
       <c r="X28" t="n">
-        <v>-0.005066999604017067</v>
+        <v>-0.01953259295246093</v>
       </c>
       <c r="Y28" t="n">
-        <v>-0.04254782387791295</v>
+        <v>-0.00727294000352241</v>
       </c>
       <c r="Z28" t="n">
-        <v>0.01723308299332332</v>
+        <v>0.00612182578087303</v>
       </c>
       <c r="AA28" t="n">
-        <v>-0.0453037024201481</v>
+        <v>-0.008731311997252479</v>
       </c>
       <c r="AB28" t="n">
-        <v>-0.0453037024201481</v>
+        <v>-0.008731311997252479</v>
       </c>
       <c r="AC28" t="n">
-        <v>-0.0453037024201481</v>
+        <v>-0.008731311997252479</v>
       </c>
       <c r="AD28" t="n">
-        <v>-0.0453037024201481</v>
+        <v>-0.008731311997252479</v>
       </c>
       <c r="AE28" t="inlineStr"/>
     </row>
@@ -3065,86 +3065,86 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>-0.01165133365005335</v>
+        <v>-0.009915452172618085</v>
       </c>
       <c r="D29" t="n">
         <v>-0.01346903641076145</v>
       </c>
       <c r="E29" t="n">
-        <v>-0.02570641974825679</v>
+        <v>-0.02524009550560382</v>
       </c>
       <c r="F29" t="n">
-        <v>0.02539382885575315</v>
+        <v>0.02539445967177838</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.01949655490812378</v>
+        <v>-0.001755685210226998</v>
       </c>
       <c r="H29" t="n">
-        <v>0.01824659400986376</v>
+        <v>0.016277274608365</v>
       </c>
       <c r="I29" t="n">
-        <v>-0.02339852167194087</v>
+        <v>-0.02346738084269523</v>
       </c>
       <c r="J29" t="n">
-        <v>-0.01712010313123384</v>
+        <v>-0.006508440668236621</v>
       </c>
       <c r="K29" t="n">
-        <v>0.01793600154944006</v>
+        <v>0.0157974101358964</v>
       </c>
       <c r="L29" t="n">
-        <v>0.01793600154944006</v>
+        <v>0.0157974101358964</v>
       </c>
       <c r="M29" t="n">
-        <v>0.01793600154944006</v>
+        <v>0.0157974101358964</v>
       </c>
       <c r="N29" t="n">
-        <v>0.01793600154944006</v>
+        <v>0.0157974101358964</v>
       </c>
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="n">
-        <v>0.02044163822566553</v>
+        <v>0.01876663035066521</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.01773308634132345</v>
+        <v>0.01563690628947625</v>
       </c>
       <c r="R29" t="n">
-        <v>0.01773308634132345</v>
+        <v>0.01563690628947625</v>
       </c>
       <c r="S29" t="n">
-        <v>0.01773308634132345</v>
+        <v>0.01563690628947625</v>
       </c>
       <c r="T29" t="n">
-        <v>0.01773308634132345</v>
+        <v>0.01563690628947625</v>
       </c>
       <c r="U29" t="n">
-        <v>-0.04187401444296057</v>
+        <v>-0.02711093801243752</v>
       </c>
       <c r="V29" t="n">
-        <v>-0.07657974632718983</v>
+        <v>-0.03498739973549598</v>
       </c>
       <c r="W29" t="n">
-        <v>0.03880943464037738</v>
+        <v>0.03889235598769424</v>
       </c>
       <c r="X29" t="n">
-        <v>-0.002180340873995988</v>
+        <v>-0.009665656205390038</v>
       </c>
       <c r="Y29" t="n">
-        <v>0.007196987903879515</v>
+        <v>0.003271834659838928</v>
       </c>
       <c r="Z29" t="n">
-        <v>0.01161849032073961</v>
+        <v>0.01903065071322603</v>
       </c>
       <c r="AA29" t="n">
-        <v>0.007032758105310323</v>
+        <v>0.002461905890476235</v>
       </c>
       <c r="AB29" t="n">
-        <v>0.007032758105310323</v>
+        <v>0.002461905890476235</v>
       </c>
       <c r="AC29" t="n">
-        <v>0.007032758105310323</v>
+        <v>0.002461905890476235</v>
       </c>
       <c r="AD29" t="n">
-        <v>0.007032758105310323</v>
+        <v>0.002461905890476235</v>
       </c>
       <c r="AE29" t="inlineStr"/>
     </row>
@@ -3160,86 +3160,86 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>-0.01621863626474545</v>
+        <v>-0.02157989865519594</v>
       </c>
       <c r="D30" t="n">
         <v>-0.02053317413332696</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.004801578528063141</v>
+        <v>-0.01407686917107476</v>
       </c>
       <c r="F30" t="n">
-        <v>0.008285351083414041</v>
+        <v>0.00828530231541209</v>
       </c>
       <c r="G30" t="n">
-        <v>9.928693538498253e-05</v>
+        <v>-0.003161036757164427</v>
       </c>
       <c r="H30" t="n">
-        <v>0.01006870792274831</v>
+        <v>0.006012371734774978</v>
       </c>
       <c r="I30" t="n">
-        <v>-0.02186607303464292</v>
+        <v>-0.02109652212386088</v>
       </c>
       <c r="J30" t="n">
-        <v>-0.01803691651439277</v>
+        <v>-0.0007714878576924178</v>
       </c>
       <c r="K30" t="n">
-        <v>0.01093421054936842</v>
+        <v>0.008431250833250033</v>
       </c>
       <c r="L30" t="n">
-        <v>0.01093421054936842</v>
+        <v>0.008431250833250033</v>
       </c>
       <c r="M30" t="n">
-        <v>0.01093421054936842</v>
+        <v>0.008431250833250033</v>
       </c>
       <c r="N30" t="n">
-        <v>0.01093421054936842</v>
+        <v>0.008431250833250033</v>
       </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="n">
-        <v>0.01010809394032376</v>
+        <v>0.009518746748749869</v>
       </c>
       <c r="Q30" t="n">
-        <v>0.01112683071707323</v>
+        <v>0.00828108551524342</v>
       </c>
       <c r="R30" t="n">
-        <v>0.01112683071707323</v>
+        <v>0.00828108551524342</v>
       </c>
       <c r="S30" t="n">
-        <v>0.01112683071707323</v>
+        <v>0.00828108551524342</v>
       </c>
       <c r="T30" t="n">
-        <v>0.01112683071707323</v>
+        <v>0.00828108551524342</v>
       </c>
       <c r="U30" t="n">
-        <v>0.006372091838883672</v>
+        <v>-0.007941150653646025</v>
       </c>
       <c r="V30" t="n">
-        <v>0.06200946180837846</v>
+        <v>-0.001834254217370169</v>
       </c>
       <c r="W30" t="n">
-        <v>0.0003856151194246047</v>
+        <v>0.0004344158573766342</v>
       </c>
       <c r="X30" t="n">
-        <v>-0.01705359387230663</v>
+        <v>-0.005026571796973453</v>
       </c>
       <c r="Y30" t="n">
-        <v>0.01988489618739584</v>
+        <v>0.01007344636966131</v>
       </c>
       <c r="Z30" t="n">
-        <v>-0.0003395139975805599</v>
+        <v>0.008036160609446423</v>
       </c>
       <c r="AA30" t="n">
-        <v>0.01290964870838594</v>
+        <v>0.007029107705164307</v>
       </c>
       <c r="AB30" t="n">
-        <v>0.01290964870838594</v>
+        <v>0.007029107705164307</v>
       </c>
       <c r="AC30" t="n">
-        <v>0.01290964870838594</v>
+        <v>0.007029107705164307</v>
       </c>
       <c r="AD30" t="n">
-        <v>0.01290964870838594</v>
+        <v>0.007029107705164307</v>
       </c>
       <c r="AE30" t="inlineStr"/>
     </row>
@@ -3255,86 +3255,86 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>-0.0009188399407535975</v>
+        <v>0.0005417201496688059</v>
       </c>
       <c r="D31" t="n">
         <v>-0.002391382367655294</v>
       </c>
       <c r="E31" t="n">
-        <v>-0.001223010480920419</v>
+        <v>0.00116070849442834</v>
       </c>
       <c r="F31" t="n">
-        <v>-0.004086688387467535</v>
+        <v>-0.004086284611451384</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.01958825558477172</v>
+        <v>0.006032650081708801</v>
       </c>
       <c r="H31" t="n">
-        <v>-0.003690020499600819</v>
+        <v>-0.004649027542618529</v>
       </c>
       <c r="I31" t="n">
-        <v>0.01270018380400735</v>
+        <v>0.01285679081827163</v>
       </c>
       <c r="J31" t="n">
-        <v>-0.005945451373942119</v>
+        <v>-0.03106268377256952</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.00305786777031471</v>
+        <v>-0.005036949801477991</v>
       </c>
       <c r="L31" t="n">
-        <v>-0.00305786777031471</v>
+        <v>-0.005036949801477991</v>
       </c>
       <c r="M31" t="n">
-        <v>-0.00305786777031471</v>
+        <v>-0.005036949801477991</v>
       </c>
       <c r="N31" t="n">
-        <v>-0.00305786777031471</v>
+        <v>-0.005036949801477991</v>
       </c>
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="n">
-        <v>-0.001847887561915502</v>
+        <v>-0.004163790982551639</v>
       </c>
       <c r="Q31" t="n">
-        <v>-0.003056189786247591</v>
+        <v>-0.004933066757322669</v>
       </c>
       <c r="R31" t="n">
-        <v>-0.003056189786247591</v>
+        <v>-0.004933066757322669</v>
       </c>
       <c r="S31" t="n">
-        <v>-0.003056189786247591</v>
+        <v>-0.004933066757322669</v>
       </c>
       <c r="T31" t="n">
-        <v>-0.003056189786247591</v>
+        <v>-0.004933066757322669</v>
       </c>
       <c r="U31" t="n">
-        <v>0.002532450629298025</v>
+        <v>-0.03040450278418011</v>
       </c>
       <c r="V31" t="n">
-        <v>-0.0008866014114640563</v>
+        <v>0.0003087089403483575</v>
       </c>
       <c r="W31" t="n">
-        <v>0.001552489886099595</v>
+        <v>0.001475352539014101</v>
       </c>
       <c r="X31" t="n">
-        <v>0.005959213525150725</v>
+        <v>-0.006919778252281826</v>
       </c>
       <c r="Y31" t="n">
-        <v>-0.01576226991049079</v>
+        <v>0.03668746099334194</v>
       </c>
       <c r="Z31" t="n">
-        <v>-0.006049129201965167</v>
+        <v>0.01531861482074459</v>
       </c>
       <c r="AA31" t="n">
-        <v>-0.01117561388702455</v>
+        <v>0.03429712178788487</v>
       </c>
       <c r="AB31" t="n">
-        <v>-0.01117561388702455</v>
+        <v>0.03429712178788487</v>
       </c>
       <c r="AC31" t="n">
-        <v>-0.01117561388702455</v>
+        <v>0.03429712178788487</v>
       </c>
       <c r="AD31" t="n">
-        <v>-0.01117561388702455</v>
+        <v>0.03429712178788487</v>
       </c>
       <c r="AE31" t="inlineStr"/>
     </row>
@@ -3350,86 +3350,86 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.4842944538997782</v>
+        <v>0.4672434662097386</v>
       </c>
       <c r="D32" t="n">
         <v>-0.001273986386959456</v>
       </c>
       <c r="E32" t="n">
-        <v>0.9873117757804709</v>
+        <v>0.9435281861891274</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.9158583885703354</v>
+        <v>-0.9158585582983422</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.03017044502999384</v>
+        <v>0.013232499286858</v>
       </c>
       <c r="H32" t="n">
-        <v>-0.8919204503648178</v>
+        <v>-0.8747433167897601</v>
       </c>
       <c r="I32" t="n">
-        <v>-0.06797797337511892</v>
+        <v>-0.06908949578757981</v>
       </c>
       <c r="J32" t="n">
-        <v>0.4195070653099857</v>
+        <v>0.3636663377700363</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.9271352843814111</v>
+        <v>-0.9086905160276205</v>
       </c>
       <c r="L32" t="n">
-        <v>-0.9271352843814111</v>
+        <v>-0.9086905160276205</v>
       </c>
       <c r="M32" t="n">
-        <v>-0.9271352843814111</v>
+        <v>-0.9086905160276205</v>
       </c>
       <c r="N32" t="n">
-        <v>-0.9271352843814111</v>
+        <v>-0.9086905160276205</v>
       </c>
       <c r="O32" t="inlineStr"/>
       <c r="P32" t="n">
-        <v>-0.9408016487040658</v>
+        <v>-0.9282090640083624</v>
       </c>
       <c r="Q32" t="n">
-        <v>-0.9225513120380523</v>
+        <v>-0.902608950248358</v>
       </c>
       <c r="R32" t="n">
-        <v>-0.9225513120380523</v>
+        <v>-0.902608950248358</v>
       </c>
       <c r="S32" t="n">
-        <v>-0.9225513120380523</v>
+        <v>-0.902608950248358</v>
       </c>
       <c r="T32" t="n">
-        <v>-0.9225513120380523</v>
+        <v>-0.902608950248358</v>
       </c>
       <c r="U32" t="n">
-        <v>-0.0666445851617834</v>
+        <v>-0.01909191877967675</v>
       </c>
       <c r="V32" t="n">
-        <v>0.004893011907720476</v>
+        <v>0.02310492351619694</v>
       </c>
       <c r="W32" t="n">
-        <v>0.02051159381246375</v>
+        <v>0.0203155399166216</v>
       </c>
       <c r="X32" t="n">
-        <v>0.03852056641057625</v>
+        <v>0.0899849698396393</v>
       </c>
       <c r="Y32" t="n">
-        <v>0.1116283157291326</v>
+        <v>0.1149324712362145</v>
       </c>
       <c r="Z32" t="n">
-        <v>-0.03681453440058138</v>
+        <v>0.008666874298674972</v>
       </c>
       <c r="AA32" t="n">
-        <v>0.5056179405767176</v>
+        <v>0.2785130746605229</v>
       </c>
       <c r="AB32" t="n">
-        <v>0.5056179405767176</v>
+        <v>0.2785130746605229</v>
       </c>
       <c r="AC32" t="n">
-        <v>0.5056179405767176</v>
+        <v>0.2785130746605229</v>
       </c>
       <c r="AD32" t="n">
-        <v>0.5056179405767176</v>
+        <v>0.2785130746605229</v>
       </c>
       <c r="AE32" t="inlineStr"/>
     </row>
@@ -3445,86 +3445,86 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.03375112531804501</v>
+        <v>0.03518392892735715</v>
       </c>
       <c r="D33" t="n">
         <v>-0.003106481884259275</v>
       </c>
       <c r="E33" t="n">
-        <v>0.05353209314928372</v>
+        <v>0.05637792619111705</v>
       </c>
       <c r="F33" t="n">
-        <v>-0.05868764337150573</v>
+        <v>-0.05869031284361251</v>
       </c>
       <c r="G33" t="n">
-        <v>0.006934342280674567</v>
+        <v>0.01996462969819824</v>
       </c>
       <c r="H33" t="n">
-        <v>-0.05454850691794027</v>
+        <v>-0.04965068009416847</v>
       </c>
       <c r="I33" t="n">
-        <v>-0.0214526227141049</v>
+        <v>-0.01870181930807277</v>
       </c>
       <c r="J33" t="n">
-        <v>0.1066015263771644</v>
+        <v>0.1202688421643809</v>
       </c>
       <c r="K33" t="n">
-        <v>-0.05426267161050686</v>
+        <v>-0.05175429346217172</v>
       </c>
       <c r="L33" t="n">
-        <v>-0.05426267161050686</v>
+        <v>-0.05175429346217172</v>
       </c>
       <c r="M33" t="n">
-        <v>-0.05426267161050686</v>
+        <v>-0.05175429346217172</v>
       </c>
       <c r="N33" t="n">
-        <v>-0.05426267161050686</v>
+        <v>-0.05175429346217172</v>
       </c>
       <c r="O33" t="inlineStr"/>
       <c r="P33" t="n">
-        <v>-0.05444622630584904</v>
+        <v>-0.05365282985811319</v>
       </c>
       <c r="Q33" t="n">
-        <v>-0.05406899400275976</v>
+        <v>-0.05119009635160385</v>
       </c>
       <c r="R33" t="n">
-        <v>-0.05406899400275976</v>
+        <v>-0.05119009635160385</v>
       </c>
       <c r="S33" t="n">
-        <v>-0.05406899400275976</v>
+        <v>-0.05119009635160385</v>
       </c>
       <c r="T33" t="n">
-        <v>-0.05406899400275976</v>
+        <v>-0.05119009635160385</v>
       </c>
       <c r="U33" t="n">
-        <v>0.005149999981999998</v>
+        <v>-0.008603385176135405</v>
       </c>
       <c r="V33" t="n">
-        <v>-0.02557525494301019</v>
+        <v>0.02097921808716872</v>
       </c>
       <c r="W33" t="n">
-        <v>-0.02615480927019237</v>
+        <v>-0.02627357855494314</v>
       </c>
       <c r="X33" t="n">
-        <v>0.02914287494871666</v>
+        <v>0.02721591203098041</v>
       </c>
       <c r="Y33" t="n">
-        <v>-0.01167724721908989</v>
+        <v>0.02374878303197017</v>
       </c>
       <c r="Z33" t="n">
-        <v>0.00548231100329244</v>
+        <v>0.01724430568177222</v>
       </c>
       <c r="AA33" t="n">
-        <v>0.01163833035353321</v>
+        <v>0.03310245866809834</v>
       </c>
       <c r="AB33" t="n">
-        <v>0.01163833035353321</v>
+        <v>0.03310245866809834</v>
       </c>
       <c r="AC33" t="n">
-        <v>0.01163833035353321</v>
+        <v>0.03310245866809834</v>
       </c>
       <c r="AD33" t="n">
-        <v>0.01163833035353321</v>
+        <v>0.03310245866809834</v>
       </c>
       <c r="AE33" t="inlineStr"/>
     </row>
@@ -3540,86 +3540,86 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.0009247645809905831</v>
+        <v>0.0007097033563881342</v>
       </c>
       <c r="D34" t="n">
         <v>0.002479635075185403</v>
       </c>
       <c r="E34" t="n">
-        <v>0.002002802672112107</v>
+        <v>0.001747389093895564</v>
       </c>
       <c r="F34" t="n">
-        <v>-0.001321499092859963</v>
+        <v>-0.00132169925286797</v>
       </c>
       <c r="G34" t="n">
-        <v>0.0114169395224465</v>
+        <v>-0.006998691655601238</v>
       </c>
       <c r="H34" t="n">
-        <v>4.321651372866054e-05</v>
+        <v>-0.0009884739049238591</v>
       </c>
       <c r="I34" t="n">
-        <v>0.01408465419538616</v>
+        <v>0.01429063170762527</v>
       </c>
       <c r="J34" t="n">
-        <v>-0.03118064283578761</v>
+        <v>-0.02461118440281965</v>
       </c>
       <c r="K34" t="n">
-        <v>0.001738834245553369</v>
+        <v>-0.0006037517041500681</v>
       </c>
       <c r="L34" t="n">
-        <v>0.001738834245553369</v>
+        <v>-0.0006037517041500681</v>
       </c>
       <c r="M34" t="n">
-        <v>0.001738834245553369</v>
+        <v>-0.0006037517041500681</v>
       </c>
       <c r="N34" t="n">
-        <v>0.001738834245553369</v>
+        <v>-0.0006037517041500681</v>
       </c>
       <c r="O34" t="inlineStr"/>
       <c r="P34" t="n">
-        <v>0.001147395597895824</v>
+        <v>-0.0007962752958510117</v>
       </c>
       <c r="Q34" t="n">
-        <v>0.00188861575554463</v>
+        <v>-0.0003604735824189432</v>
       </c>
       <c r="R34" t="n">
-        <v>0.00188861575554463</v>
+        <v>-0.0003604735824189432</v>
       </c>
       <c r="S34" t="n">
-        <v>0.00188861575554463</v>
+        <v>-0.0003604735824189432</v>
       </c>
       <c r="T34" t="n">
-        <v>0.00188861575554463</v>
+        <v>-0.0003604735824189432</v>
       </c>
       <c r="U34" t="n">
-        <v>-0.01033599804543992</v>
+        <v>-0.01539404231176169</v>
       </c>
       <c r="V34" t="n">
-        <v>-0.01057749901509996</v>
+        <v>0.0009930245197209806</v>
       </c>
       <c r="W34" t="n">
-        <v>-0.001261884722475389</v>
+        <v>-0.001416145688645827</v>
       </c>
       <c r="X34" t="n">
-        <v>-0.01661065547696289</v>
+        <v>0.02969661995960157</v>
       </c>
       <c r="Y34" t="n">
-        <v>-0.0008968813798752551</v>
+        <v>0.01722126585868089</v>
       </c>
       <c r="Z34" t="n">
-        <v>0.01851297914051916</v>
+        <v>0.02143930300157212</v>
       </c>
       <c r="AA34" t="n">
-        <v>-0.001729689381187575</v>
+        <v>0.01639665137586606</v>
       </c>
       <c r="AB34" t="n">
-        <v>-0.001729689381187575</v>
+        <v>0.01639665137586606</v>
       </c>
       <c r="AC34" t="n">
-        <v>-0.001729689381187575</v>
+        <v>0.01639665137586606</v>
       </c>
       <c r="AD34" t="n">
-        <v>-0.001729689381187575</v>
+        <v>0.01639665137586606</v>
       </c>
       <c r="AE34" t="inlineStr"/>
     </row>
@@ -3635,86 +3635,86 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>-0.03363370838534833</v>
+        <v>-0.02772553090102124</v>
       </c>
       <c r="D35" t="n">
         <v>0.007347835109913403</v>
       </c>
       <c r="E35" t="n">
-        <v>-0.03095121215004848</v>
+        <v>-0.01962457268898291</v>
       </c>
       <c r="F35" t="n">
-        <v>0.01786464973858599</v>
+        <v>0.01786503114660124</v>
       </c>
       <c r="G35" t="n">
-        <v>0.006036595745901797</v>
+        <v>-0.01280319937645925</v>
       </c>
       <c r="H35" t="n">
-        <v>0.01719084385563375</v>
+        <v>0.02184173520846947</v>
       </c>
       <c r="I35" t="n">
-        <v>0.008064809794592389</v>
+        <v>0.00813603430944137</v>
       </c>
       <c r="J35" t="n">
-        <v>-0.01099128469345975</v>
+        <v>-0.008328344811715474</v>
       </c>
       <c r="K35" t="n">
-        <v>0.05350983382039335</v>
+        <v>0.05496060901442435</v>
       </c>
       <c r="L35" t="n">
-        <v>0.05350983382039335</v>
+        <v>0.05496060901442435</v>
       </c>
       <c r="M35" t="n">
-        <v>0.05350983382039335</v>
+        <v>0.05496060901442435</v>
       </c>
       <c r="N35" t="n">
-        <v>0.05350983382039335</v>
+        <v>0.05496060901442435</v>
       </c>
       <c r="O35" t="inlineStr"/>
       <c r="P35" t="n">
-        <v>0.04959435452777418</v>
+        <v>0.05018686098347443</v>
       </c>
       <c r="Q35" t="n">
-        <v>0.05430253762810149</v>
+        <v>0.05594087311763492</v>
       </c>
       <c r="R35" t="n">
-        <v>0.05430253762810149</v>
+        <v>0.05594087311763492</v>
       </c>
       <c r="S35" t="n">
-        <v>0.05430253762810149</v>
+        <v>0.05594087311763492</v>
       </c>
       <c r="T35" t="n">
-        <v>0.05430253762810149</v>
+        <v>0.05594087311763492</v>
       </c>
       <c r="U35" t="n">
-        <v>-0.003776468983058759</v>
+        <v>0.01678416201536648</v>
       </c>
       <c r="V35" t="n">
-        <v>-0.02229370476374819</v>
+        <v>0.01665730319429212</v>
       </c>
       <c r="W35" t="n">
-        <v>-0.02884743907389756</v>
+        <v>-0.02879706067188242</v>
       </c>
       <c r="X35" t="n">
-        <v>-0.01243528698543266</v>
+        <v>0.01313616681275606</v>
       </c>
       <c r="Y35" t="n">
-        <v>-0.02677098817483952</v>
+        <v>-0.02509318364678014</v>
       </c>
       <c r="Z35" t="n">
-        <v>0.02776592808663712</v>
+        <v>0.004137416421496656</v>
       </c>
       <c r="AA35" t="n">
-        <v>-0.04039010676760426</v>
+        <v>-0.03401038446441538</v>
       </c>
       <c r="AB35" t="n">
-        <v>-0.04039010676760426</v>
+        <v>-0.03401038446441538</v>
       </c>
       <c r="AC35" t="n">
-        <v>-0.04039010676760426</v>
+        <v>-0.03401038446441538</v>
       </c>
       <c r="AD35" t="n">
-        <v>-0.04039010676760426</v>
+        <v>-0.03401038446441538</v>
       </c>
       <c r="AE35" t="inlineStr"/>
     </row>
@@ -3730,86 +3730,86 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>-0.01106139634645585</v>
+        <v>-0.009858664138346565</v>
       </c>
       <c r="D36" t="n">
         <v>-0.005466936218677448</v>
       </c>
       <c r="E36" t="n">
-        <v>0.01565639889825595</v>
+        <v>0.01508586338743453</v>
       </c>
       <c r="F36" t="n">
-        <v>-0.01583263532130541</v>
+        <v>-0.01583363324134533</v>
       </c>
       <c r="G36" t="n">
-        <v>-5.715098758850323e-05</v>
+        <v>0.01886857189649572</v>
       </c>
       <c r="H36" t="n">
-        <v>-0.01112805894112236</v>
+        <v>-0.01146270789475811</v>
       </c>
       <c r="I36" t="n">
-        <v>0.002162695190507808</v>
+        <v>0.001515725052629002</v>
       </c>
       <c r="J36" t="n">
-        <v>0.03054160714449312</v>
+        <v>0.01197670799504679</v>
       </c>
       <c r="K36" t="n">
-        <v>-0.01165042971401719</v>
+        <v>-0.01165802091432084</v>
       </c>
       <c r="L36" t="n">
-        <v>-0.01165042971401719</v>
+        <v>-0.01165802091432084</v>
       </c>
       <c r="M36" t="n">
-        <v>-0.01165042971401719</v>
+        <v>-0.01165802091432084</v>
       </c>
       <c r="N36" t="n">
-        <v>-0.01165042971401719</v>
+        <v>-0.01165802091432084</v>
       </c>
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="n">
-        <v>-0.01270279558011182</v>
+        <v>-0.01285793955431758</v>
       </c>
       <c r="Q36" t="n">
-        <v>-0.01141214772048591</v>
+        <v>-0.01152293450891738</v>
       </c>
       <c r="R36" t="n">
-        <v>-0.01141214772048591</v>
+        <v>-0.01152293450891738</v>
       </c>
       <c r="S36" t="n">
-        <v>-0.01141214772048591</v>
+        <v>-0.01152293450891738</v>
       </c>
       <c r="T36" t="n">
-        <v>-0.01141214772048591</v>
+        <v>-0.01152293450891738</v>
       </c>
       <c r="U36" t="n">
-        <v>0.02716355811054232</v>
+        <v>0.0240319226892769</v>
       </c>
       <c r="V36" t="n">
-        <v>0.01096096027843841</v>
+        <v>0.00692334728493389</v>
       </c>
       <c r="W36" t="n">
-        <v>-0.01359679830387193</v>
+        <v>-0.01361145299245812</v>
       </c>
       <c r="X36" t="n">
-        <v>-0.007276471229951413</v>
+        <v>0.01328642759237281</v>
       </c>
       <c r="Y36" t="n">
-        <v>-0.008791498143659924</v>
+        <v>-0.000604581833405565</v>
       </c>
       <c r="Z36" t="n">
-        <v>-0.007694068435762736</v>
+        <v>-0.01657107435884297</v>
       </c>
       <c r="AA36" t="n">
-        <v>-0.01205130153805206</v>
+        <v>-0.004981106407244256</v>
       </c>
       <c r="AB36" t="n">
-        <v>-0.01205130153805206</v>
+        <v>-0.004981106407244256</v>
       </c>
       <c r="AC36" t="n">
-        <v>-0.01205130153805206</v>
+        <v>-0.004981106407244256</v>
       </c>
       <c r="AD36" t="n">
-        <v>-0.01205130153805206</v>
+        <v>-0.004981106407244256</v>
       </c>
       <c r="AE36" t="inlineStr"/>
     </row>
@@ -3825,86 +3825,86 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.0002670606826824273</v>
+        <v>-0.0009815875592635022</v>
       </c>
       <c r="D37" t="n">
         <v>0.01341683295267332</v>
       </c>
       <c r="E37" t="n">
-        <v>0.001266827378673095</v>
+        <v>-0.004401766928070676</v>
       </c>
       <c r="F37" t="n">
-        <v>0.006256305754252229</v>
+        <v>0.006256723450268937</v>
       </c>
       <c r="G37" t="n">
-        <v>0.01069609925017153</v>
+        <v>-0.006995598683024611</v>
       </c>
       <c r="H37" t="n">
-        <v>0.00699243176769727</v>
+        <v>0.005735473212249703</v>
       </c>
       <c r="I37" t="n">
-        <v>0.02672095306883812</v>
+        <v>0.02710910815636432</v>
       </c>
       <c r="J37" t="n">
-        <v>-0.003997972442761399</v>
+        <v>0.01193941900141831</v>
       </c>
       <c r="K37" t="n">
-        <v>0.009484684987387399</v>
+        <v>0.00981533050461322</v>
       </c>
       <c r="L37" t="n">
-        <v>0.009484684987387399</v>
+        <v>0.00981533050461322</v>
       </c>
       <c r="M37" t="n">
-        <v>0.009484684987387399</v>
+        <v>0.00981533050461322</v>
       </c>
       <c r="N37" t="n">
-        <v>0.009484684987387399</v>
+        <v>0.00981533050461322</v>
       </c>
       <c r="O37" t="inlineStr"/>
       <c r="P37" t="n">
-        <v>0.008143904389756176</v>
+        <v>0.008541218933648757</v>
       </c>
       <c r="Q37" t="n">
-        <v>0.009935831245433249</v>
+        <v>0.009937274029490959</v>
       </c>
       <c r="R37" t="n">
-        <v>0.009935831245433249</v>
+        <v>0.009937274029490959</v>
       </c>
       <c r="S37" t="n">
-        <v>0.009935831245433249</v>
+        <v>0.009937274029490959</v>
       </c>
       <c r="T37" t="n">
-        <v>0.009935831245433249</v>
+        <v>0.009937274029490959</v>
       </c>
       <c r="U37" t="n">
-        <v>0.006324086460963457</v>
+        <v>-0.001166994478679779</v>
       </c>
       <c r="V37" t="n">
-        <v>-0.001443678393747136</v>
+        <v>-0.0164580125623205</v>
       </c>
       <c r="W37" t="n">
-        <v>0.01890933685237347</v>
+        <v>0.01903961308158452</v>
       </c>
       <c r="X37" t="n">
-        <v>-0.002932718473463062</v>
+        <v>-0.01276877855568752</v>
       </c>
       <c r="Y37" t="n">
-        <v>-0.02339449907977996</v>
+        <v>-0.01279591720426031</v>
       </c>
       <c r="Z37" t="n">
-        <v>-0.0005324876372995054</v>
+        <v>-0.01776406170256247</v>
       </c>
       <c r="AA37" t="n">
-        <v>-0.01327300526692021</v>
+        <v>-0.008762844542513781</v>
       </c>
       <c r="AB37" t="n">
-        <v>-0.01327300526692021</v>
+        <v>-0.008762844542513781</v>
       </c>
       <c r="AC37" t="n">
-        <v>-0.01327300526692021</v>
+        <v>-0.008762844542513781</v>
       </c>
       <c r="AD37" t="n">
-        <v>-0.01327300526692021</v>
+        <v>-0.008762844542513781</v>
       </c>
       <c r="AE37" t="inlineStr"/>
     </row>
@@ -3920,86 +3920,86 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.002122805844912233</v>
+        <v>0.001805164872206595</v>
       </c>
       <c r="D38" t="n">
         <v>0.02909218925968757</v>
       </c>
       <c r="E38" t="n">
-        <v>-0.01864712205788488</v>
+        <v>-0.01515299724611989</v>
       </c>
       <c r="F38" t="n">
-        <v>0.009684142179365687</v>
+        <v>0.009683619459344777</v>
       </c>
       <c r="G38" t="n">
-        <v>0.00532386831741302</v>
+        <v>-0.03174783116429901</v>
       </c>
       <c r="H38" t="n">
-        <v>0.01150522970820919</v>
+        <v>0.01545722745903982</v>
       </c>
       <c r="I38" t="n">
-        <v>0.009905767596230701</v>
+        <v>0.01061863674474547</v>
       </c>
       <c r="J38" t="n">
-        <v>0.0009395938001319304</v>
+        <v>0.007757029394764988</v>
       </c>
       <c r="K38" t="n">
-        <v>0.01448865129954605</v>
+        <v>0.01795584407823376</v>
       </c>
       <c r="L38" t="n">
-        <v>0.01448865129954605</v>
+        <v>0.01795584407823376</v>
       </c>
       <c r="M38" t="n">
-        <v>0.01448865129954605</v>
+        <v>0.01795584407823376</v>
       </c>
       <c r="N38" t="n">
-        <v>0.01448865129954605</v>
+        <v>0.01795584407823376</v>
       </c>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="n">
-        <v>0.0152212674568507</v>
+        <v>0.01759834092793364</v>
       </c>
       <c r="Q38" t="n">
-        <v>0.01448068435522737</v>
+        <v>0.01796401819056073</v>
       </c>
       <c r="R38" t="n">
-        <v>0.01448068435522737</v>
+        <v>0.01796401819056073</v>
       </c>
       <c r="S38" t="n">
-        <v>0.01448068435522737</v>
+        <v>0.01796401819056073</v>
       </c>
       <c r="T38" t="n">
-        <v>0.01448068435522737</v>
+        <v>0.01796401819056073</v>
       </c>
       <c r="U38" t="n">
-        <v>0.009760413126416524</v>
+        <v>0.01240000619200025</v>
       </c>
       <c r="V38" t="n">
-        <v>-0.01162977963319118</v>
+        <v>-0.004714786460591458</v>
       </c>
       <c r="W38" t="n">
-        <v>0.00512160327686413</v>
+        <v>0.005174165678966627</v>
       </c>
       <c r="X38" t="n">
-        <v>0.0172171085558736</v>
+        <v>0.01805266262941733</v>
       </c>
       <c r="Y38" t="n">
-        <v>-0.01856584163863366</v>
+        <v>-0.01043287133481307</v>
       </c>
       <c r="Z38" t="n">
-        <v>-0.001937615885504635</v>
+        <v>-0.02608474885138995</v>
       </c>
       <c r="AA38" t="n">
-        <v>-0.02227891337115653</v>
+        <v>-0.01529239673969587</v>
       </c>
       <c r="AB38" t="n">
-        <v>-0.02227891337115653</v>
+        <v>-0.01529239673969587</v>
       </c>
       <c r="AC38" t="n">
-        <v>-0.02227891337115653</v>
+        <v>-0.01529239673969587</v>
       </c>
       <c r="AD38" t="n">
-        <v>-0.02227891337115653</v>
+        <v>-0.01529239673969587</v>
       </c>
       <c r="AE38" t="inlineStr"/>
     </row>
@@ -4015,86 +4015,86 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.01078707892748316</v>
+        <v>0.004902707236108288</v>
       </c>
       <c r="D39" t="n">
         <v>0.009771227334849092</v>
       </c>
       <c r="E39" t="n">
-        <v>0.001614831904593276</v>
+        <v>-0.008129534053181361</v>
       </c>
       <c r="F39" t="n">
-        <v>-0.005167455566698222</v>
+        <v>-0.005166420302656811</v>
       </c>
       <c r="G39" t="n">
-        <v>0.0311973649194502</v>
+        <v>0.01186522016560601</v>
       </c>
       <c r="H39" t="n">
-        <v>-0.01084047441761897</v>
+        <v>-0.01473930810730038</v>
       </c>
       <c r="I39" t="n">
-        <v>-0.001403203544128142</v>
+        <v>-0.001676998819079953</v>
       </c>
       <c r="J39" t="n">
-        <v>-0.0104586321747091</v>
+        <v>-0.02715399872186943</v>
       </c>
       <c r="K39" t="n">
-        <v>0.00189691725987669</v>
+        <v>-0.001105335404213416</v>
       </c>
       <c r="L39" t="n">
-        <v>0.00189691725987669</v>
+        <v>-0.001105335404213416</v>
       </c>
       <c r="M39" t="n">
-        <v>0.00189691725987669</v>
+        <v>-0.001105335404213416</v>
       </c>
       <c r="N39" t="n">
-        <v>0.00189691725987669</v>
+        <v>-0.001105335404213416</v>
       </c>
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="n">
-        <v>0.001623399904935996</v>
+        <v>-0.0001235480689419227</v>
       </c>
       <c r="Q39" t="n">
-        <v>0.002012071568482862</v>
+        <v>-0.001328943701157748</v>
       </c>
       <c r="R39" t="n">
-        <v>0.002012071568482862</v>
+        <v>-0.001328943701157748</v>
       </c>
       <c r="S39" t="n">
-        <v>0.002012071568482862</v>
+        <v>-0.001328943701157748</v>
       </c>
       <c r="T39" t="n">
-        <v>0.002012071568482862</v>
+        <v>-0.001328943701157748</v>
       </c>
       <c r="U39" t="n">
-        <v>0.0137239176689567</v>
+        <v>-0.02120974846438993</v>
       </c>
       <c r="V39" t="n">
-        <v>0.008541944309677772</v>
+        <v>-0.02714199622167985</v>
       </c>
       <c r="W39" t="n">
-        <v>-0.0008142958405718334</v>
+        <v>-0.0007491283499651339</v>
       </c>
       <c r="X39" t="n">
-        <v>-0.02154876269661839</v>
+        <v>-0.005215353789073674</v>
       </c>
       <c r="Y39" t="n">
-        <v>0.001997437423897496</v>
+        <v>0.02691750599656094</v>
       </c>
       <c r="Z39" t="n">
-        <v>0.01580507333620293</v>
+        <v>0.0346221927768877</v>
       </c>
       <c r="AA39" t="n">
-        <v>-0.03889881246795249</v>
+        <v>0.005933938317357531</v>
       </c>
       <c r="AB39" t="n">
-        <v>-0.03889881246795249</v>
+        <v>0.005933938317357531</v>
       </c>
       <c r="AC39" t="n">
-        <v>-0.03889881246795249</v>
+        <v>0.005933938317357531</v>
       </c>
       <c r="AD39" t="n">
-        <v>-0.03889881246795249</v>
+        <v>0.005933938317357531</v>
       </c>
       <c r="AE39" t="inlineStr"/>
     </row>

</xml_diff>